<commit_message>
BOM and Machine.h file
</commit_message>
<xml_diff>
--- a/Hardware/Dring Heath Small/BOM LCSC.xlsx
+++ b/Hardware/Dring Heath Small/BOM LCSC.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c62116b6853fd2b9/Documents/CNC-Plasma-Table/Dring Heath Controller/Kicad/Dring Heath Small/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Hardware\Dring Heath Small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DC9C13E-5530-4CDE-B188-8639864E5599}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5179223A-9F19-45B9-8ADE-3BB7D673E556}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="195">
   <si>
     <t>Package</t>
   </si>
@@ -225,9 +225,6 @@
     <t>J16,J17,J18,J19,J20,J21</t>
   </si>
   <si>
-    <t>RJ45</t>
-  </si>
-  <si>
     <t>JP1,JP3,JP4</t>
   </si>
   <si>
@@ -570,9 +567,6 @@
     <t>2685Y-112CNG1SNA01</t>
   </si>
   <si>
-    <t>C124416</t>
-  </si>
-  <si>
     <t>C124411</t>
   </si>
   <si>
@@ -612,15 +606,6 @@
     <t>2x05 pin header</t>
   </si>
   <si>
-    <t>C265320</t>
-  </si>
-  <si>
-    <t>RF-H102TD-1190(LF)(SN)</t>
-  </si>
-  <si>
-    <t>RJ45_OST_PJ012-8P8CX_Vertical 2x05 pin header</t>
-  </si>
-  <si>
     <t>C239356</t>
   </si>
   <si>
@@ -637,6 +622,21 @@
   </si>
   <si>
     <t>Through Hole Ethernet Connectors/Modular Connectors (RJ45</t>
+  </si>
+  <si>
+    <t>Heade Jumper</t>
+  </si>
+  <si>
+    <t>C100114</t>
+  </si>
+  <si>
+    <t>Motor conn</t>
+  </si>
+  <si>
+    <t>C124387</t>
+  </si>
+  <si>
+    <t>C27438</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +1100,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CF0671-FE26-4F07-89AC-F4C1AA2B534B}">
-  <dimension ref="A2:N57"/>
+  <dimension ref="A2:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="O50" sqref="O50"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1119,25 +1119,25 @@
   <sheetData>
     <row r="2" spans="1:11">
       <c r="B2" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" t="s">
         <v>98</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>99</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>100</v>
       </c>
-      <c r="J2" t="s">
-        <v>101</v>
-      </c>
       <c r="K2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1166,10 +1166,10 @@
         <v>4</v>
       </c>
       <c r="I3" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>131</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>132</v>
       </c>
       <c r="K3">
         <v>50</v>
@@ -1201,10 +1201,10 @@
         <v>4</v>
       </c>
       <c r="I4" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="J4" s="11" t="s">
         <v>133</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>134</v>
       </c>
       <c r="K4">
         <v>25</v>
@@ -1236,10 +1236,10 @@
         <v>4</v>
       </c>
       <c r="I5" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="J5" s="11" t="s">
         <v>129</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>130</v>
       </c>
       <c r="K5">
         <v>20</v>
@@ -1271,10 +1271,10 @@
         <v>4</v>
       </c>
       <c r="I6" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J6" s="11" t="s">
         <v>135</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>136</v>
       </c>
       <c r="K6">
         <v>10</v>
@@ -1306,10 +1306,10 @@
         <v>4</v>
       </c>
       <c r="I7" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="J7" s="12" t="s">
         <v>137</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>138</v>
       </c>
       <c r="K7">
         <v>20</v>
@@ -1341,10 +1341,10 @@
         <v>4</v>
       </c>
       <c r="I8" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="J8" s="10" t="s">
         <v>139</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>140</v>
       </c>
       <c r="K8">
         <v>20</v>
@@ -1376,10 +1376,10 @@
         <v>4</v>
       </c>
       <c r="I9" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="J9" s="11" t="s">
         <v>141</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>142</v>
       </c>
       <c r="K9">
         <v>20</v>
@@ -1437,10 +1437,10 @@
         <v>4</v>
       </c>
       <c r="I11" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="J11" s="11" t="s">
         <v>170</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>171</v>
       </c>
       <c r="K11">
         <v>25</v>
@@ -1524,10 +1524,10 @@
         <v>4</v>
       </c>
       <c r="I14" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="J14" s="10" t="s">
         <v>145</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>146</v>
       </c>
       <c r="K14">
         <v>6</v>
@@ -1671,7 +1671,7 @@
         <v>45</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -1689,19 +1689,19 @@
         <v>4</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K20">
         <v>6</v>
       </c>
       <c r="M20" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1808,10 +1808,10 @@
         <v>4</v>
       </c>
       <c r="I24" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="J24" s="11" t="s">
         <v>166</v>
-      </c>
-      <c r="J24" s="11" t="s">
-        <v>167</v>
       </c>
       <c r="K24">
         <v>4</v>
@@ -1825,13 +1825,13 @@
         <v>56</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="D25" s="2">
         <v>6</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>57</v>
+        <v>192</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>4</v>
@@ -1843,16 +1843,16 @@
         <v>4</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="K25">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="M25" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1860,7 +1860,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>41</v>
@@ -1869,7 +1869,7 @@
         <v>3</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F26" s="7" t="s">
         <v>4</v>
@@ -1886,7 +1886,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>41</v>
@@ -1895,7 +1895,7 @@
         <v>1</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>4</v>
@@ -1912,16 +1912,16 @@
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>62</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>63</v>
       </c>
       <c r="D28" s="4">
         <v>2</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F28" s="7" t="s">
         <v>4</v>
@@ -1933,10 +1933,10 @@
         <v>4</v>
       </c>
       <c r="I28" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="J28" s="11" t="s">
         <v>147</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>148</v>
       </c>
       <c r="K28">
         <v>10</v>
@@ -1947,16 +1947,16 @@
         <v>27</v>
       </c>
       <c r="B29" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F29" s="5" t="s">
         <v>4</v>
@@ -1973,17 +1973,17 @@
         <v>28</v>
       </c>
       <c r="B30" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="D30" s="4">
+        <v>4</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D30" s="4">
-        <v>4</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>70</v>
-      </c>
       <c r="F30" s="7" t="s">
         <v>4</v>
       </c>
@@ -1994,10 +1994,10 @@
         <v>4</v>
       </c>
       <c r="I30" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="J30" s="10" t="s">
         <v>153</v>
-      </c>
-      <c r="J30" s="10" t="s">
-        <v>154</v>
       </c>
       <c r="K30">
         <v>50</v>
@@ -2008,17 +2008,17 @@
         <v>29</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D31" s="2">
-        <v>4</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="F31" s="5" t="s">
         <v>4</v>
       </c>
@@ -2029,10 +2029,10 @@
         <v>4</v>
       </c>
       <c r="I31" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="J31" s="11" t="s">
         <v>151</v>
-      </c>
-      <c r="J31" s="11" t="s">
-        <v>152</v>
       </c>
       <c r="K31">
         <v>40</v>
@@ -2043,16 +2043,16 @@
         <v>30</v>
       </c>
       <c r="B32" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="D32" s="4">
         <v>2</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F32" s="7" t="s">
         <v>4</v>
@@ -2064,10 +2064,10 @@
         <v>4</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K32">
         <v>15</v>
@@ -2078,17 +2078,17 @@
         <v>31</v>
       </c>
       <c r="B33" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="D33" s="2">
+        <v>1</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D33" s="2">
-        <v>1</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="F33" s="5" t="s">
         <v>4</v>
       </c>
@@ -2099,10 +2099,10 @@
         <v>4</v>
       </c>
       <c r="I33" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="J33" s="11" t="s">
         <v>155</v>
-      </c>
-      <c r="J33" s="11" t="s">
-        <v>156</v>
       </c>
       <c r="K33">
         <v>5</v>
@@ -2113,17 +2113,17 @@
         <v>32</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="4">
+        <v>1</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="4">
-        <v>1</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>80</v>
-      </c>
       <c r="F34" s="7" t="s">
         <v>4</v>
       </c>
@@ -2134,10 +2134,10 @@
         <v>4</v>
       </c>
       <c r="I34" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="J34" s="11" t="s">
         <v>157</v>
-      </c>
-      <c r="J34" s="11" t="s">
-        <v>158</v>
       </c>
       <c r="K34">
         <v>5</v>
@@ -2148,17 +2148,17 @@
         <v>33</v>
       </c>
       <c r="B35" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="D35" s="2">
+        <v>4</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D35" s="2">
-        <v>4</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="F35" s="5" t="s">
         <v>4</v>
       </c>
@@ -2169,10 +2169,10 @@
         <v>4</v>
       </c>
       <c r="I35" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="J35" s="11" t="s">
         <v>159</v>
-      </c>
-      <c r="J35" s="11" t="s">
-        <v>160</v>
       </c>
       <c r="K35">
         <v>15</v>
@@ -2183,17 +2183,17 @@
         <v>34</v>
       </c>
       <c r="B36" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="D36" s="4">
+        <v>1</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="D36" s="4">
-        <v>1</v>
-      </c>
-      <c r="E36" s="7" t="s">
-        <v>86</v>
-      </c>
       <c r="F36" s="7" t="s">
         <v>4</v>
       </c>
@@ -2204,16 +2204,16 @@
         <v>4</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="K36">
         <v>40</v>
       </c>
       <c r="L36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -2221,17 +2221,17 @@
         <v>35</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="2">
+        <v>1</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D37" s="2">
-        <v>1</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="F37" s="5" t="s">
         <v>4</v>
       </c>
@@ -2242,16 +2242,16 @@
         <v>4</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K37">
         <v>15</v>
       </c>
       <c r="L37" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -2259,16 +2259,16 @@
         <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="4">
+        <v>1</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D38" s="4">
-        <v>1</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>4</v>
@@ -2285,16 +2285,16 @@
         <v>37</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>91</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D39" s="2">
-        <v>1</v>
-      </c>
-      <c r="E39" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>4</v>
@@ -2311,16 +2311,16 @@
         <v>38</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="4">
+        <v>1</v>
+      </c>
+      <c r="E40" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D40" s="4">
-        <v>1</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>4</v>
@@ -2337,16 +2337,16 @@
         <v>39</v>
       </c>
       <c r="B41" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="2">
+        <v>1</v>
+      </c>
+      <c r="E41" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D41" s="2">
-        <v>1</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>96</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>4</v>
@@ -2361,7 +2361,7 @@
     <row r="42" spans="1:13">
       <c r="A42" s="1"/>
       <c r="B42" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="2"/>
@@ -2375,16 +2375,16 @@
         <v>1</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>189</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="D43" s="2">
-        <v>1</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>103</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>4</v>
@@ -2398,7 +2398,7 @@
       <c r="I43" s="11"/>
       <c r="J43" s="11"/>
       <c r="M43" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -2406,16 +2406,16 @@
         <v>2</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D44" s="4">
         <v>6</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F44" s="7" t="s">
         <v>4</v>
@@ -2432,7 +2432,7 @@
         <v>3</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>2</v>
@@ -2441,7 +2441,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>4</v>
@@ -2453,10 +2453,10 @@
         <v>4</v>
       </c>
       <c r="I45" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J45" s="11" t="s">
         <v>127</v>
-      </c>
-      <c r="J45" s="11" t="s">
-        <v>128</v>
       </c>
       <c r="K45">
         <v>20</v>
@@ -2467,7 +2467,7 @@
         <v>4</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>2</v>
@@ -2476,7 +2476,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>4</v>
@@ -2496,14 +2496,14 @@
         <v>10</v>
       </c>
       <c r="C47" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D47" s="2">
-        <v>1</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>110</v>
-      </c>
       <c r="F47" s="5" t="s">
         <v>4</v>
       </c>
@@ -2514,10 +2514,10 @@
         <v>4</v>
       </c>
       <c r="I47" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="J47" s="11" t="s">
         <v>143</v>
-      </c>
-      <c r="J47" s="11" t="s">
-        <v>144</v>
       </c>
       <c r="K47">
         <v>50</v>
@@ -2531,13 +2531,13 @@
         <v>25</v>
       </c>
       <c r="C48" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" s="4">
+        <v>1</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="D48" s="4">
-        <v>1</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>4</v>
@@ -2554,17 +2554,17 @@
         <v>7</v>
       </c>
       <c r="B49" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="D49" s="2">
+        <v>1</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D49" s="2">
-        <v>1</v>
-      </c>
-      <c r="E49" s="5" t="s">
-        <v>115</v>
-      </c>
       <c r="F49" s="5" t="s">
         <v>4</v>
       </c>
@@ -2575,16 +2575,16 @@
         <v>4</v>
       </c>
       <c r="I49" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="J49" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="J49" s="11" t="s">
+      <c r="K49">
+        <v>4</v>
+      </c>
+      <c r="L49" t="s">
         <v>162</v>
-      </c>
-      <c r="K49">
-        <v>4</v>
-      </c>
-      <c r="L49" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -2592,17 +2592,17 @@
         <v>8</v>
       </c>
       <c r="B50" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="D50" s="4">
+        <v>1</v>
+      </c>
+      <c r="E50" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="D50" s="4">
-        <v>1</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>118</v>
-      </c>
       <c r="F50" s="7" t="s">
         <v>4</v>
       </c>
@@ -2613,10 +2613,10 @@
         <v>4</v>
       </c>
       <c r="I50" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="J50" s="11" t="s">
         <v>168</v>
-      </c>
-      <c r="J50" s="11" t="s">
-        <v>169</v>
       </c>
       <c r="K50">
         <v>20</v>
@@ -2627,16 +2627,16 @@
         <v>9</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D51" s="2">
         <v>2</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F51" s="5" t="s">
         <v>4</v>
@@ -2653,16 +2653,16 @@
         <v>10</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D52" s="4">
         <v>2</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>4</v>
@@ -2674,10 +2674,10 @@
         <v>4</v>
       </c>
       <c r="I52" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="J52" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="J52" s="11" t="s">
-        <v>150</v>
       </c>
       <c r="K52">
         <v>50</v>
@@ -2691,13 +2691,13 @@
         <v>28</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D53" s="2">
         <v>1</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>4</v>
@@ -2714,17 +2714,17 @@
         <v>12</v>
       </c>
       <c r="B54" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C54" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="D54" s="4">
+        <v>1</v>
+      </c>
+      <c r="E54" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="D54" s="4">
-        <v>1</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>125</v>
-      </c>
       <c r="F54" s="7" t="s">
         <v>4</v>
       </c>
@@ -2735,10 +2735,10 @@
         <v>4</v>
       </c>
       <c r="I54" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="J54" s="11" t="s">
         <v>164</v>
-      </c>
-      <c r="J54" s="11" t="s">
-        <v>165</v>
       </c>
       <c r="K54">
         <v>15</v>
@@ -2746,13 +2746,13 @@
     </row>
     <row r="55" spans="1:12">
       <c r="C55" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="I55" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="J55" s="10" t="s">
         <v>182</v>
-      </c>
-      <c r="I55" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="J55" s="10" t="s">
-        <v>184</v>
       </c>
       <c r="K55">
         <v>10</v>
@@ -2760,13 +2760,13 @@
     </row>
     <row r="56" spans="1:12">
       <c r="C56" s="14" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I56" s="11" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="K56">
         <v>20</v>
@@ -2774,7 +2774,21 @@
     </row>
     <row r="57" spans="1:12">
       <c r="C57" s="13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12">
+      <c r="C58" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="I58" s="11" t="s">
         <v>191</v>
+      </c>
+      <c r="J58" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="K58">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2818,21 +2832,23 @@
     <hyperlink ref="J50" r:id="rId37" display="https://lcsc.com/product-detail/MOSFET_Changjiang-Electronics-Tech-CJ-BSS138_C78284.html" xr:uid="{FC024E6B-4477-41A4-8F13-D235177224EA}"/>
     <hyperlink ref="I11" r:id="rId38" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_HOAUC-2685Y-112CNG1SNA01_C350303.html" xr:uid="{5ED41FCA-2D62-4C8C-A2CA-36B7F0F8B1EA}"/>
     <hyperlink ref="J11" r:id="rId39" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_HOAUC-2685Y-112CNG1SNA01_C350303.html" xr:uid="{1BB65DA6-8F70-45D7-ADC9-31E73153A346}"/>
-    <hyperlink ref="I36" r:id="rId40" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-Female-header-1-8P-2-54mm-Straight-line_C124416.html" xr:uid="{4B5518E6-6A68-48AE-B82C-3941D24741D1}"/>
-    <hyperlink ref="J36" r:id="rId41" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-Female-header-1-8P-2-54mm-Straight-line_C124416.html" xr:uid="{120D961E-1337-4A68-B5D8-78D5C809202E}"/>
-    <hyperlink ref="I37" r:id="rId42" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-Female-header-1-2P-2-54mm-Straight-line_C124411.html" xr:uid="{00473F31-1536-4EF6-B88D-F04B05003259}"/>
-    <hyperlink ref="J37" r:id="rId43" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-Female-header-1-2P-2-54mm-Straight-line_C124411.html" xr:uid="{5C5F4AB7-A56B-4D9C-8DD0-AB6C3DD1A382}"/>
-    <hyperlink ref="I20" r:id="rId44" display="https://lcsc.com/product-detail/New-Arrivals_PINREX-510-80-10GB43_C390693.html" xr:uid="{ECAA16D5-B7C0-4006-AF8D-EAA603F805A8}"/>
-    <hyperlink ref="J20" r:id="rId45" display="https://lcsc.com/product-detail/New-Arrivals_PINREX-510-80-10GB43_C390693.html" xr:uid="{94E02D6B-5943-42FD-A204-8ADE9E505276}"/>
-    <hyperlink ref="I32" r:id="rId46" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-C124418_C124418.html" xr:uid="{B98456FE-8FAF-41B0-9FC8-F2307B6A0EBC}"/>
-    <hyperlink ref="J32" r:id="rId47" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-C124418_C124418.html" xr:uid="{7A591889-3641-4B21-8F90-72B2714D314A}"/>
-    <hyperlink ref="I55" r:id="rId48" display="https://lcsc.com/product-detail/Ethernet-Connectors-Modular-Connectors-RJ45-RJ11_Amphenol-ICC-RJHSE5380_C464586.html" xr:uid="{2E52DB74-83EC-476B-A2F7-5A24CA8F1D8C}"/>
-    <hyperlink ref="I25" r:id="rId49" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_JST-Sales-America-RF-H102TD-1190-LF-SN_C265320.html" xr:uid="{4769BEE3-AC9C-4237-99E5-236D34AF66AD}"/>
-    <hyperlink ref="J25" r:id="rId50" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_JST-Sales-America-RF-H102TD-1190-LF-SN_C265320.html" xr:uid="{AD13D499-4130-40D5-9670-5B29D67F4B80}"/>
-    <hyperlink ref="I56" r:id="rId51" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_CJT-Changjiang-Connectors-A2541HWR-2x5P_C239356.html" xr:uid="{3DA55EE5-2E64-4035-AFFF-1173D2D34C1E}"/>
+    <hyperlink ref="J36" r:id="rId40" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-Female-header-1-8P-2-54mm-Straight-line_C124416.html" xr:uid="{120D961E-1337-4A68-B5D8-78D5C809202E}"/>
+    <hyperlink ref="I37" r:id="rId41" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-Female-header-1-2P-2-54mm-Straight-line_C124411.html" xr:uid="{00473F31-1536-4EF6-B88D-F04B05003259}"/>
+    <hyperlink ref="J37" r:id="rId42" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-Female-header-1-2P-2-54mm-Straight-line_C124411.html" xr:uid="{5C5F4AB7-A56B-4D9C-8DD0-AB6C3DD1A382}"/>
+    <hyperlink ref="I20" r:id="rId43" display="https://lcsc.com/product-detail/New-Arrivals_PINREX-510-80-10GB43_C390693.html" xr:uid="{ECAA16D5-B7C0-4006-AF8D-EAA603F805A8}"/>
+    <hyperlink ref="J20" r:id="rId44" display="https://lcsc.com/product-detail/New-Arrivals_PINREX-510-80-10GB43_C390693.html" xr:uid="{94E02D6B-5943-42FD-A204-8ADE9E505276}"/>
+    <hyperlink ref="I32" r:id="rId45" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-C124418_C124418.html" xr:uid="{B98456FE-8FAF-41B0-9FC8-F2307B6A0EBC}"/>
+    <hyperlink ref="J32" r:id="rId46" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-C124418_C124418.html" xr:uid="{7A591889-3641-4B21-8F90-72B2714D314A}"/>
+    <hyperlink ref="I55" r:id="rId47" display="https://lcsc.com/product-detail/Ethernet-Connectors-Modular-Connectors-RJ45-RJ11_Amphenol-ICC-RJHSE5380_C464586.html" xr:uid="{2E52DB74-83EC-476B-A2F7-5A24CA8F1D8C}"/>
+    <hyperlink ref="I25" r:id="rId48" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_JST-Sales-America-RF-H102TD-1190-LF-SN_C265320.html" xr:uid="{4769BEE3-AC9C-4237-99E5-236D34AF66AD}"/>
+    <hyperlink ref="I56" r:id="rId49" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_CJT-Changjiang-Connectors-A2541HWR-2x5P_C239356.html" xr:uid="{3DA55EE5-2E64-4035-AFFF-1173D2D34C1E}"/>
+    <hyperlink ref="I58" r:id="rId50" display="https://lcsc.com/product-detail/Shunts-Jumpers_BOOMELE-Boom-Precision-Elec-C100114_C100114.html" xr:uid="{F5944AA6-6EFB-4D49-8C41-4C3AE1679B09}"/>
+    <hyperlink ref="J58" r:id="rId51" display="https://lcsc.com/product-detail/Shunts-Jumpers_BOOMELE-Boom-Precision-Elec-C100114_C100114.html" xr:uid="{3B986909-AB08-4903-9FC2-4ED0C15097DF}"/>
+    <hyperlink ref="J25" r:id="rId52" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-Headers-Pins-2-5P-2-54mm-Straight-line_C124387.html" xr:uid="{C8C02C2D-AB0B-49A6-8D2F-B364B37C3B93}"/>
+    <hyperlink ref="I36" r:id="rId53" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_BOOMELE-Boom-Precision-Elec-2-54mm-1-8P-Straight-Female-header_C27438.html" xr:uid="{8CFF675A-5B77-4C96-937A-D09D917A58EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId52"/>
+  <pageSetup orientation="portrait" r:id="rId54"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added files to Grbl_Esp32 for VScode
</commit_message>
<xml_diff>
--- a/Hardware/Dring Heath Small/BOM LCSC.xlsx
+++ b/Hardware/Dring Heath Small/BOM LCSC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Hardware\Dring Heath Small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B31CB36-99FB-488D-9B00-D7FE75717DCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC75CF2-C239-49E1-A21C-A82E41ABDD33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
+    <workbookView xWindow="31005" yWindow="1875" windowWidth="20280" windowHeight="12885" activeTab="1" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="306">
   <si>
     <t>Package</t>
   </si>
@@ -961,6 +961,15 @@
   </si>
   <si>
     <t>GPIO12</t>
+  </si>
+  <si>
+    <t>TrimPot 20K</t>
+  </si>
+  <si>
+    <t>3266W-1-203</t>
+  </si>
+  <si>
+    <t>C124983</t>
   </si>
 </sst>
 </file>
@@ -1442,7 +1451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823C39F3-7594-4535-810B-0496FC455A11}">
   <dimension ref="B1:O81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="N74" sqref="N74"/>
     </sheetView>
   </sheetViews>
@@ -2719,10 +2728,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CF0671-FE26-4F07-89AC-F4C1AA2B534B}">
-  <dimension ref="A2:N58"/>
+  <dimension ref="A2:N59"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J54" sqref="J54"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="K64" sqref="K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4408,6 +4417,20 @@
       </c>
       <c r="K58">
         <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="C59" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="J59" s="11" t="s">
+        <v>304</v>
+      </c>
+      <c r="K59">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4465,9 +4488,11 @@
     <hyperlink ref="J58" r:id="rId51" display="https://lcsc.com/product-detail/Shunts-Jumpers_BOOMELE-Boom-Precision-Elec-C100114_C100114.html" xr:uid="{3B986909-AB08-4903-9FC2-4ED0C15097DF}"/>
     <hyperlink ref="J25" r:id="rId52" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-Headers-Pins-2-5P-2-54mm-Straight-line_C124387.html" xr:uid="{C8C02C2D-AB0B-49A6-8D2F-B364B37C3B93}"/>
     <hyperlink ref="I36" r:id="rId53" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_BOOMELE-Boom-Precision-Elec-2-54mm-1-8P-Straight-Female-header_C27438.html" xr:uid="{8CFF675A-5B77-4C96-937A-D09D917A58EF}"/>
+    <hyperlink ref="J59" r:id="rId54" display="https://lcsc.com/product-detail/Precision-Potentiometer_BOCHEN-Chengdu-Guosheng-Tech-3266W-1-203_C124983.html" xr:uid="{CA13AF68-61FC-4064-89E2-34536F2B755A}"/>
+    <hyperlink ref="I59" r:id="rId55" display="https://lcsc.com/product-detail/Precision-Potentiometer_BOCHEN-Chengdu-Guosheng-Tech-3266W-1-203_C124983.html" xr:uid="{405AF7DC-500C-411C-94B4-9E4DA3BD5513}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId54"/>
+  <pageSetup orientation="portrait" r:id="rId56"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added mosfet motor driver
</commit_message>
<xml_diff>
--- a/Hardware/Dring Heath Small/BOM LCSC.xlsx
+++ b/Hardware/Dring Heath Small/BOM LCSC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Hardware\Dring Heath Small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A623AE1D-CC3F-447B-BA3A-CEA00C2FF414}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7E5E559-31CB-4F1E-B85B-ECDF52545A24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31005" yWindow="1875" windowWidth="20280" windowHeight="12885" activeTab="1" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
+    <workbookView xWindow="30825" yWindow="1200" windowWidth="20280" windowHeight="12885" activeTab="1" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="311">
   <si>
     <t>Package</t>
   </si>
@@ -288,6 +288,12 @@
     <t>U4</t>
   </si>
   <si>
+    <t>SOT-223</t>
+  </si>
+  <si>
+    <t>TC1262-33</t>
+  </si>
+  <si>
     <t>U5,U6,U7,U8</t>
   </si>
   <si>
@@ -399,9 +405,6 @@
     <t>SOT-23</t>
   </si>
   <si>
-    <t>AO3400A</t>
-  </si>
-  <si>
     <t>R2,R9</t>
   </si>
   <si>
@@ -516,6 +519,12 @@
     <t>XL74LS157</t>
   </si>
   <si>
+    <t>C52507</t>
+  </si>
+  <si>
+    <t>TC1262-3.3VDBTR</t>
+  </si>
+  <si>
     <t>C503428</t>
   </si>
   <si>
@@ -543,12 +552,6 @@
     <t>DM3AT-SF-PEJM5</t>
   </si>
   <si>
-    <t>C78284</t>
-  </si>
-  <si>
-    <t>BSS138</t>
-  </si>
-  <si>
     <t>C350303</t>
   </si>
   <si>
@@ -951,25 +954,37 @@
     <t>GPIO12</t>
   </si>
   <si>
-    <t>TrimPot 20K</t>
-  </si>
-  <si>
-    <t>3266W-1-203</t>
-  </si>
-  <si>
-    <t>C124983</t>
-  </si>
-  <si>
-    <t>C401677</t>
-  </si>
-  <si>
-    <t>BL8071CLATR33</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SOT-223</t>
-  </si>
-  <si>
-    <t>BL8071 3.3v Reg</t>
+    <t>SOP-8</t>
+  </si>
+  <si>
+    <t>Dual mosfet</t>
+  </si>
+  <si>
+    <t>SE4942B</t>
+  </si>
+  <si>
+    <t>C238652</t>
+  </si>
+  <si>
+    <t>IRLML2402</t>
+  </si>
+  <si>
+    <t>C475705</t>
+  </si>
+  <si>
+    <t>Nchannel mosfet</t>
+  </si>
+  <si>
+    <t>SMD 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200 ohm </t>
+  </si>
+  <si>
+    <t>ERJPA3F2000V</t>
+  </si>
+  <si>
+    <t>C254528</t>
   </si>
 </sst>
 </file>
@@ -1451,7 +1466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823C39F3-7594-4535-810B-0496FC455A11}">
   <dimension ref="B1:O81"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="N74" sqref="N74"/>
     </sheetView>
   </sheetViews>
@@ -1502,37 +1517,37 @@
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F4" t="s">
         <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="J4" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>27</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="O4" s="15"/>
     </row>
@@ -1547,10 +1562,10 @@
     </row>
     <row r="6" spans="2:15">
       <c r="B6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="J6" s="16"/>
       <c r="K6" s="15"/>
@@ -1561,7 +1576,7 @@
     </row>
     <row r="7" spans="2:15">
       <c r="B7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I7" s="15"/>
       <c r="J7" s="16">
@@ -1577,26 +1592,26 @@
     </row>
     <row r="8" spans="2:15">
       <c r="B8" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C8" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D8">
         <v>34</v>
       </c>
       <c r="G8" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="16">
         <v>2</v>
       </c>
       <c r="K8" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L8" s="15"/>
       <c r="M8" s="15"/>
@@ -1605,14 +1620,14 @@
     </row>
     <row r="9" spans="2:15">
       <c r="B9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I9" s="15"/>
       <c r="J9" s="16">
         <v>3</v>
       </c>
       <c r="K9" s="15" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
@@ -1621,10 +1636,10 @@
     </row>
     <row r="10" spans="2:15">
       <c r="B10" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C10" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D10">
         <v>26</v>
@@ -1633,14 +1648,14 @@
         <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I10" s="15"/>
       <c r="J10" s="16">
         <v>4</v>
       </c>
       <c r="K10" s="15" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L10" s="15"/>
       <c r="M10" s="15"/>
@@ -1649,91 +1664,91 @@
     </row>
     <row r="11" spans="2:15">
       <c r="B11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C11" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E11">
         <v>32</v>
       </c>
       <c r="G11" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H11" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="J11" s="16">
         <v>5</v>
       </c>
       <c r="K11" s="15" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="M11" s="15" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="O11" s="15"/>
     </row>
     <row r="12" spans="2:15">
       <c r="B12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C12" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D12" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E12">
         <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="J12" s="16">
         <v>6</v>
       </c>
       <c r="K12" s="15" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="M12" s="15" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="N12" s="15" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="O12" s="15"/>
     </row>
     <row r="13" spans="2:15">
       <c r="B13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E13">
         <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="H13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="I13" s="15"/>
       <c r="J13" s="16">
@@ -1743,29 +1758,29 @@
       <c r="L13" s="15"/>
       <c r="M13" s="15"/>
       <c r="N13" s="15" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="O13" s="15"/>
     </row>
     <row r="14" spans="2:15">
       <c r="B14" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C14" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E14">
         <v>22</v>
       </c>
       <c r="G14" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I14" s="15"/>
       <c r="J14" s="16">
         <v>8</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L14" s="15"/>
       <c r="M14" s="15"/>
@@ -1774,42 +1789,42 @@
     </row>
     <row r="15" spans="2:15">
       <c r="B15" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C15" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="D15" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E15">
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="16"/>
       <c r="K15" s="15"/>
       <c r="L15" s="15"/>
       <c r="M15" s="15" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
     </row>
     <row r="16" spans="2:15">
       <c r="B16" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="J16" s="16">
         <v>1</v>
       </c>
       <c r="K16" s="15" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L16" s="15"/>
       <c r="M16" s="16">
@@ -1820,14 +1835,14 @@
     </row>
     <row r="17" spans="2:15">
       <c r="B17" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="I17" s="15"/>
       <c r="J17" s="16">
         <v>2</v>
       </c>
       <c r="K17" s="15" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="L17" s="15"/>
       <c r="M17" s="16">
@@ -1838,14 +1853,14 @@
     </row>
     <row r="18" spans="2:15">
       <c r="B18" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="I18" s="15"/>
       <c r="J18" s="16">
         <v>3</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L18" s="15"/>
       <c r="M18" s="16">
@@ -1856,20 +1871,20 @@
     </row>
     <row r="19" spans="2:15">
       <c r="B19" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E19">
         <v>32</v>
       </c>
       <c r="G19" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I19" s="15"/>
       <c r="J19" s="16">
         <v>4</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L19" s="15"/>
       <c r="M19" s="16">
@@ -1880,13 +1895,13 @@
     </row>
     <row r="20" spans="2:15">
       <c r="B20" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E20">
         <v>19</v>
       </c>
       <c r="G20" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I20" s="15"/>
       <c r="J20" s="16">
@@ -1900,7 +1915,7 @@
     </row>
     <row r="21" spans="2:15">
       <c r="B21" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I21" s="15"/>
       <c r="J21" s="16">
@@ -1914,7 +1929,7 @@
     </row>
     <row r="22" spans="2:15">
       <c r="B22" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="I22" s="15"/>
       <c r="J22" s="16">
@@ -1932,16 +1947,16 @@
     </row>
     <row r="23" spans="2:15">
       <c r="B23" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="J23" s="16">
         <v>8</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L23" s="15"/>
       <c r="M23" s="16">
@@ -1961,13 +1976,13 @@
     </row>
     <row r="25" spans="2:15">
       <c r="I25" s="15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J25" s="16">
         <v>1</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L25" s="15"/>
       <c r="M25" s="15"/>
@@ -1993,7 +2008,7 @@
         <v>3</v>
       </c>
       <c r="K27" s="15" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="L27" s="15"/>
       <c r="M27" s="15"/>
@@ -2010,10 +2025,10 @@
       </c>
       <c r="L28" s="15"/>
       <c r="M28" s="15" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="N28" s="15" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="O28" s="15"/>
     </row>
@@ -2025,7 +2040,7 @@
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
       <c r="M29" s="15" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="N29" s="15"/>
       <c r="O29" s="15"/>
@@ -2038,27 +2053,27 @@
       <c r="K30" s="15"/>
       <c r="L30" s="15"/>
       <c r="M30" s="15" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="N30" s="15"/>
       <c r="O30" s="15"/>
     </row>
     <row r="31" spans="2:15">
       <c r="I31" s="15" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="J31" s="16">
         <v>7</v>
       </c>
       <c r="K31" s="15" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="L31" s="15"/>
       <c r="M31" s="15" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="N31" s="15" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="O31" s="15"/>
     </row>
@@ -2068,14 +2083,14 @@
         <v>8</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L32" s="15"/>
       <c r="M32" s="15" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="N32" s="15" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="O32" s="15"/>
     </row>
@@ -2089,10 +2104,10 @@
       </c>
       <c r="L33" s="15"/>
       <c r="M33" s="15" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="O33" s="15"/>
     </row>
@@ -2102,12 +2117,12 @@
         <v>10</v>
       </c>
       <c r="K34" s="15" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
       <c r="N34" s="15" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="O34" s="15"/>
     </row>
@@ -2117,12 +2132,12 @@
         <v>11</v>
       </c>
       <c r="K35" s="15" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="L35" s="15"/>
       <c r="M35" s="15"/>
       <c r="N35" s="15" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="O35" s="15"/>
     </row>
@@ -2132,7 +2147,7 @@
         <v>12</v>
       </c>
       <c r="K36" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L36" s="15"/>
       <c r="M36" s="15"/>
@@ -2159,7 +2174,7 @@
     </row>
     <row r="39" spans="9:15">
       <c r="I39" s="15" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="J39" s="16">
         <v>1</v>
@@ -2178,7 +2193,7 @@
         <v>2</v>
       </c>
       <c r="K40" s="15" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
@@ -2204,7 +2219,7 @@
         <v>4</v>
       </c>
       <c r="K42" s="15" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
@@ -2230,7 +2245,7 @@
         <v>6</v>
       </c>
       <c r="K44" s="15" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
@@ -2256,7 +2271,7 @@
         <v>8</v>
       </c>
       <c r="K46" s="15" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
@@ -2269,7 +2284,7 @@
         <v>9</v>
       </c>
       <c r="K47" s="15" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
@@ -2282,7 +2297,7 @@
         <v>10</v>
       </c>
       <c r="K48" s="15" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
@@ -2300,7 +2315,7 @@
     </row>
     <row r="50" spans="9:15">
       <c r="I50" s="15" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J50" s="16">
         <v>1</v>
@@ -2319,10 +2334,10 @@
         <v>2</v>
       </c>
       <c r="K51" s="15" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L51" s="15" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
@@ -2347,10 +2362,10 @@
         <v>6</v>
       </c>
       <c r="K53" s="15" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="L53" s="15" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
@@ -2359,10 +2374,10 @@
     <row r="54" spans="9:15">
       <c r="I54" s="15"/>
       <c r="J54" s="16" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="K54" s="15" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
@@ -2380,13 +2395,13 @@
     </row>
     <row r="56" spans="9:15">
       <c r="I56" s="15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J56" s="16">
         <v>1</v>
       </c>
       <c r="K56" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L56" s="15"/>
       <c r="M56" s="15"/>
@@ -2412,7 +2427,7 @@
         <v>6</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
@@ -2425,7 +2440,7 @@
         <v>7</v>
       </c>
       <c r="K59" s="15" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
@@ -2438,7 +2453,7 @@
         <v>12</v>
       </c>
       <c r="K60" s="15" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
@@ -2456,13 +2471,13 @@
     </row>
     <row r="62" spans="9:15">
       <c r="I62" s="15" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J62" s="16">
         <v>1</v>
       </c>
       <c r="K62" s="15" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="L62" s="15"/>
       <c r="M62" s="15"/>
@@ -2475,7 +2490,7 @@
         <v>2</v>
       </c>
       <c r="K63" s="15" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="L63" s="15"/>
       <c r="M63" s="15"/>
@@ -2488,7 +2503,7 @@
         <v>3</v>
       </c>
       <c r="K64" s="15" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L64" s="15"/>
       <c r="M64" s="15"/>
@@ -2501,7 +2516,7 @@
         <v>4</v>
       </c>
       <c r="K65" s="15" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
@@ -2514,7 +2529,7 @@
         <v>5</v>
       </c>
       <c r="K66" s="15" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="L66" s="15"/>
       <c r="M66" s="15"/>
@@ -2527,7 +2542,7 @@
         <v>6</v>
       </c>
       <c r="K67" s="15" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="L67" s="15"/>
       <c r="M67" s="15"/>
@@ -2540,7 +2555,7 @@
         <v>7</v>
       </c>
       <c r="K68" s="15" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="L68" s="15"/>
       <c r="M68" s="15"/>
@@ -2553,7 +2568,7 @@
         <v>8</v>
       </c>
       <c r="K69" s="15" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L69" s="15"/>
       <c r="M69" s="15"/>
@@ -2571,7 +2586,7 @@
     </row>
     <row r="71" spans="9:15">
       <c r="I71" s="15" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="J71" s="16">
         <v>1</v>
@@ -2580,7 +2595,7 @@
         <v>21</v>
       </c>
       <c r="L71" s="15" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M71" s="15"/>
       <c r="N71" s="15"/>
@@ -2592,10 +2607,10 @@
         <v>2</v>
       </c>
       <c r="K72" s="15" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="L72" s="15" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="M72" s="15"/>
       <c r="N72" s="15"/>
@@ -2607,10 +2622,10 @@
         <v>3</v>
       </c>
       <c r="K73" s="15" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L73" s="15" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="M73" s="15"/>
       <c r="N73" s="15"/>
@@ -2622,10 +2637,10 @@
         <v>4</v>
       </c>
       <c r="K74" s="15" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="L74" s="15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M74" s="15"/>
       <c r="N74" s="15"/>
@@ -2637,10 +2652,10 @@
         <v>5</v>
       </c>
       <c r="K75" s="15" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L75" s="15" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="M75" s="15"/>
       <c r="N75" s="15"/>
@@ -2652,10 +2667,10 @@
         <v>6</v>
       </c>
       <c r="K76" s="15" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="L76" s="15" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M76" s="15"/>
       <c r="N76" s="15"/>
@@ -2667,10 +2682,10 @@
         <v>8</v>
       </c>
       <c r="K77" s="15" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="L77" s="15" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="M77" s="15"/>
       <c r="N77" s="15"/>
@@ -2682,10 +2697,10 @@
         <v>9</v>
       </c>
       <c r="K78" s="15" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L78" s="15" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="M78" s="15"/>
       <c r="N78" s="15"/>
@@ -2728,10 +2743,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CF0671-FE26-4F07-89AC-F4C1AA2B534B}">
-  <dimension ref="A2:N59"/>
+  <dimension ref="A2:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2747,25 +2762,25 @@
   <sheetData>
     <row r="2" spans="1:11">
       <c r="B2" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I2" t="s">
+        <v>99</v>
+      </c>
+      <c r="J2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" t="s">
         <v>97</v>
-      </c>
-      <c r="J2" t="s">
-        <v>98</v>
-      </c>
-      <c r="K2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2794,10 +2809,10 @@
         <v>4</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="K3">
         <v>50</v>
@@ -2829,10 +2844,10 @@
         <v>4</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K4">
         <v>25</v>
@@ -2864,10 +2879,10 @@
         <v>4</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K5">
         <v>20</v>
@@ -2899,10 +2914,10 @@
         <v>4</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K6">
         <v>10</v>
@@ -2934,10 +2949,10 @@
         <v>4</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="K7">
         <v>20</v>
@@ -2969,10 +2984,10 @@
         <v>4</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K8">
         <v>20</v>
@@ -3004,10 +3019,10 @@
         <v>4</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="K9">
         <v>20</v>
@@ -3065,10 +3080,10 @@
         <v>4</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="K11">
         <v>25</v>
@@ -3152,10 +3167,10 @@
         <v>4</v>
       </c>
       <c r="I14" s="11" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K14">
         <v>6</v>
@@ -3299,7 +3314,7 @@
         <v>45</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D20" s="4">
         <v>1</v>
@@ -3317,19 +3332,19 @@
         <v>4</v>
       </c>
       <c r="I20" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J20" s="11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K20">
         <v>6</v>
       </c>
       <c r="M20" t="s">
+        <v>175</v>
+      </c>
+      <c r="N20" t="s">
         <v>174</v>
-      </c>
-      <c r="N20" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -3436,10 +3451,10 @@
         <v>4</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="J24" s="11" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="K24">
         <v>4</v>
@@ -3453,13 +3468,13 @@
         <v>56</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D25" s="2">
         <v>6</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F25" s="5" t="s">
         <v>4</v>
@@ -3471,16 +3486,16 @@
         <v>4</v>
       </c>
       <c r="I25" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="J25" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K25">
         <v>30</v>
       </c>
       <c r="M25" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -3561,10 +3576,10 @@
         <v>4</v>
       </c>
       <c r="I28" s="11" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="K28">
         <v>10</v>
@@ -3622,13 +3637,13 @@
         <v>4</v>
       </c>
       <c r="I30" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J30" s="10" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K30">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -3657,13 +3672,13 @@
         <v>4</v>
       </c>
       <c r="I31" s="11" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="J31" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K31">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -3692,10 +3707,10 @@
         <v>4</v>
       </c>
       <c r="I32" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="J32" s="11" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="K32">
         <v>15</v>
@@ -3727,10 +3742,10 @@
         <v>4</v>
       </c>
       <c r="I33" s="11" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J33" s="11" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K33">
         <v>5</v>
@@ -3744,22 +3759,28 @@
         <v>77</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>304</v>
+        <v>78</v>
       </c>
       <c r="D34" s="4">
         <v>1</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="8"/>
+        <v>79</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="I34" s="11" t="s">
-        <v>302</v>
+        <v>155</v>
       </c>
       <c r="J34" s="11" t="s">
-        <v>303</v>
+        <v>156</v>
       </c>
       <c r="K34">
         <v>5</v>
@@ -3770,16 +3791,16 @@
         <v>33</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D35" s="2">
         <v>4</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>4</v>
@@ -3791,10 +3812,10 @@
         <v>4</v>
       </c>
       <c r="I35" s="11" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="J35" s="11" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="K35">
         <v>15</v>
@@ -3805,16 +3826,16 @@
         <v>34</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D36" s="4">
         <v>1</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F36" s="7" t="s">
         <v>4</v>
@@ -3826,16 +3847,16 @@
         <v>4</v>
       </c>
       <c r="I36" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="J36" s="11" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="K36">
         <v>40</v>
       </c>
       <c r="L36" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -3843,16 +3864,16 @@
         <v>35</v>
       </c>
       <c r="B37" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="D37" s="2">
         <v>1</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F37" s="5" t="s">
         <v>4</v>
@@ -3864,16 +3885,16 @@
         <v>4</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="J37" s="11" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="K37">
         <v>15</v>
       </c>
       <c r="L37" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -3881,16 +3902,16 @@
         <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D38" s="4">
         <v>1</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="F38" s="7" t="s">
         <v>4</v>
@@ -3907,16 +3928,16 @@
         <v>37</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D39" s="2">
         <v>1</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>4</v>
@@ -3933,16 +3954,16 @@
         <v>38</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D40" s="4">
         <v>1</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="F40" s="7" t="s">
         <v>4</v>
@@ -3959,16 +3980,16 @@
         <v>39</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D41" s="2">
         <v>1</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>4</v>
@@ -3983,7 +4004,7 @@
     <row r="42" spans="1:13">
       <c r="A42" s="1"/>
       <c r="B42" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="2"/>
@@ -3997,16 +4018,16 @@
         <v>1</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D43" s="2">
         <v>1</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="F43" s="5" t="s">
         <v>4</v>
@@ -4020,7 +4041,7 @@
       <c r="I43" s="11"/>
       <c r="J43" s="11"/>
       <c r="M43" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -4028,7 +4049,7 @@
         <v>2</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>68</v>
@@ -4054,7 +4075,7 @@
         <v>3</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>2</v>
@@ -4063,7 +4084,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="F45" s="5" t="s">
         <v>4</v>
@@ -4075,10 +4096,10 @@
         <v>4</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J45" s="11" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="K45">
         <v>20</v>
@@ -4089,7 +4110,7 @@
         <v>4</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>2</v>
@@ -4098,7 +4119,7 @@
         <v>1</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="F46" s="7" t="s">
         <v>4</v>
@@ -4118,13 +4139,13 @@
         <v>10</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D47" s="2">
         <v>1</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="F47" s="5" t="s">
         <v>4</v>
@@ -4136,10 +4157,10 @@
         <v>4</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J47" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K47">
         <v>50</v>
@@ -4153,13 +4174,13 @@
         <v>25</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D48" s="4">
         <v>1</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="F48" s="7" t="s">
         <v>4</v>
@@ -4176,16 +4197,16 @@
         <v>7</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D49" s="2">
         <v>1</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F49" s="5" t="s">
         <v>4</v>
@@ -4197,16 +4218,16 @@
         <v>4</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="J49" s="11" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="K49">
         <v>4</v>
       </c>
       <c r="L49" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -4214,16 +4235,16 @@
         <v>8</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D50" s="4">
         <v>1</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>115</v>
+        <v>306</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>4</v>
@@ -4235,10 +4256,10 @@
         <v>4</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>163</v>
+        <v>305</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>164</v>
+        <v>304</v>
       </c>
       <c r="K50">
         <v>20</v>
@@ -4249,7 +4270,7 @@
         <v>9</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>68</v>
@@ -4275,7 +4296,7 @@
         <v>10</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>68</v>
@@ -4284,7 +4305,7 @@
         <v>2</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="F52" s="7" t="s">
         <v>4</v>
@@ -4296,10 +4317,10 @@
         <v>4</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="K52">
         <v>50</v>
@@ -4313,13 +4334,13 @@
         <v>28</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D53" s="2">
         <v>1</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F53" s="5" t="s">
         <v>4</v>
@@ -4336,16 +4357,16 @@
         <v>12</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D54" s="4">
         <v>1</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F54" s="7" t="s">
         <v>4</v>
@@ -4357,10 +4378,10 @@
         <v>4</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="J54" s="11" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="K54">
         <v>15</v>
@@ -4368,13 +4389,13 @@
     </row>
     <row r="55" spans="1:12">
       <c r="C55" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J55" s="10" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="K55">
         <v>10</v>
@@ -4382,13 +4403,13 @@
     </row>
     <row r="56" spans="1:12">
       <c r="C56" s="14" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I56" s="11" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J56" s="10" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="K56">
         <v>20</v>
@@ -4396,18 +4417,18 @@
     </row>
     <row r="57" spans="1:12">
       <c r="C57" s="13" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="58" spans="1:12">
       <c r="C58" s="13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="I58" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="J58" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K58">
         <v>50</v>
@@ -4415,16 +4436,33 @@
     </row>
     <row r="59" spans="1:12">
       <c r="C59" s="13" t="s">
-        <v>299</v>
+        <v>300</v>
+      </c>
+      <c r="E59" t="s">
+        <v>301</v>
       </c>
       <c r="I59" s="11" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="J59" s="11" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="K59">
-        <v>10</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12">
+      <c r="C60" t="s">
+        <v>307</v>
+      </c>
+      <c r="E60" t="s">
+        <v>308</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>310</v>
+      </c>
+      <c r="J60" s="11" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -4455,15 +4493,15 @@
     <hyperlink ref="I30" r:id="rId24" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJ3GEYJ103V_C169849.html" xr:uid="{C88F6E48-D997-4C1A-B45D-0E1A80304A7B}"/>
     <hyperlink ref="I33" r:id="rId25" display="https://lcsc.com/product-detail/Signal-Switches-Multiplexers-Decoders_XINLUDA-XL74LS157_C707097.html" xr:uid="{F90840E3-D203-479C-A250-17D178183B21}"/>
     <hyperlink ref="J33" r:id="rId26" display="https://lcsc.com/product-detail/Signal-Switches-Multiplexers-Decoders_XINLUDA-XL74LS157_C707097.html" xr:uid="{F638D2A2-DF4A-4403-9950-8FC9182755CC}"/>
-    <hyperlink ref="I35" r:id="rId27" display="https://lcsc.com/product-detail/Shift-Registers_Nexperia-74AHCT595D-118_C503428.html" xr:uid="{C6E5F93F-F0AA-4BD7-83CC-4F5F70557D35}"/>
-    <hyperlink ref="J35" r:id="rId28" display="https://lcsc.com/product-detail/Shift-Registers_Nexperia-74AHCT595D-118_C503428.html" xr:uid="{BD6E1B8A-CD13-4B06-B53D-2FEE0F5A5E5A}"/>
-    <hyperlink ref="I49" r:id="rId29" display="https://lcsc.com/product-detail/Relays_Omron-Electronics-G6E-134P-ST-US-DC12_C469134.html" xr:uid="{EFA4044B-EAEA-4F7A-A220-BA39A4E15CE9}"/>
-    <hyperlink ref="J49" r:id="rId30" display="https://lcsc.com/product-detail/Relays_Omron-Electronics-G6E-134P-ST-US-DC12_C469134.html" xr:uid="{5FA2FB73-4677-4AA9-B86A-08A677D1C62D}"/>
-    <hyperlink ref="J54" r:id="rId31" display="https://lcsc.com/product-detail/Darlington-transistor-array-driver_STMicroelectronics-ULN2003D1013TR_C61273.html" xr:uid="{5CF51D98-8AB8-4E82-9915-B25730C45FED}"/>
-    <hyperlink ref="I24" r:id="rId32" display="https://lcsc.com/product-detail/Card-Sockets-Connectors_HRS-Hirose-DM3AT-SF-PEJM5_C114218.html" xr:uid="{51EDCF0D-1E50-4AF6-8D38-BCFEDF0B131F}"/>
-    <hyperlink ref="J24" r:id="rId33" display="https://lcsc.com/product-detail/Card-Sockets-Connectors_HRS-Hirose-DM3AT-SF-PEJM5_C114218.html" xr:uid="{AFC712D9-006E-418A-8E61-FB743FDBF9CF}"/>
-    <hyperlink ref="I50" r:id="rId34" display="https://lcsc.com/product-detail/MOSFET_Changjiang-Electronics-Tech-CJ-BSS138_C78284.html" xr:uid="{0B630362-3033-4A10-A2AD-4C3E5E7EE4DD}"/>
-    <hyperlink ref="J50" r:id="rId35" display="https://lcsc.com/product-detail/MOSFET_Changjiang-Electronics-Tech-CJ-BSS138_C78284.html" xr:uid="{FC024E6B-4477-41A4-8F13-D235177224EA}"/>
+    <hyperlink ref="I34" r:id="rId27" display="https://lcsc.com/product-detail/Dropout-Regulators-LDO_Microchip-Tech-TC1262-3-3VDBTR_C52507.html" xr:uid="{97219DEA-4DE2-4D80-B72D-518E85A9C984}"/>
+    <hyperlink ref="J34" r:id="rId28" display="https://lcsc.com/product-detail/Dropout-Regulators-LDO_Microchip-Tech-TC1262-3-3VDBTR_C52507.html" xr:uid="{BA53A359-24A8-43EC-A07B-2011CA6DBC20}"/>
+    <hyperlink ref="I35" r:id="rId29" display="https://lcsc.com/product-detail/Shift-Registers_Nexperia-74AHCT595D-118_C503428.html" xr:uid="{C6E5F93F-F0AA-4BD7-83CC-4F5F70557D35}"/>
+    <hyperlink ref="J35" r:id="rId30" display="https://lcsc.com/product-detail/Shift-Registers_Nexperia-74AHCT595D-118_C503428.html" xr:uid="{BD6E1B8A-CD13-4B06-B53D-2FEE0F5A5E5A}"/>
+    <hyperlink ref="I49" r:id="rId31" display="https://lcsc.com/product-detail/Relays_Omron-Electronics-G6E-134P-ST-US-DC12_C469134.html" xr:uid="{EFA4044B-EAEA-4F7A-A220-BA39A4E15CE9}"/>
+    <hyperlink ref="J49" r:id="rId32" display="https://lcsc.com/product-detail/Relays_Omron-Electronics-G6E-134P-ST-US-DC12_C469134.html" xr:uid="{5FA2FB73-4677-4AA9-B86A-08A677D1C62D}"/>
+    <hyperlink ref="J54" r:id="rId33" display="https://lcsc.com/product-detail/Darlington-transistor-array-driver_STMicroelectronics-ULN2003D1013TR_C61273.html" xr:uid="{5CF51D98-8AB8-4E82-9915-B25730C45FED}"/>
+    <hyperlink ref="I24" r:id="rId34" display="https://lcsc.com/product-detail/Card-Sockets-Connectors_HRS-Hirose-DM3AT-SF-PEJM5_C114218.html" xr:uid="{51EDCF0D-1E50-4AF6-8D38-BCFEDF0B131F}"/>
+    <hyperlink ref="J24" r:id="rId35" display="https://lcsc.com/product-detail/Card-Sockets-Connectors_HRS-Hirose-DM3AT-SF-PEJM5_C114218.html" xr:uid="{AFC712D9-006E-418A-8E61-FB743FDBF9CF}"/>
     <hyperlink ref="I11" r:id="rId36" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_HOAUC-2685Y-112CNG1SNA01_C350303.html" xr:uid="{5ED41FCA-2D62-4C8C-A2CA-36B7F0F8B1EA}"/>
     <hyperlink ref="J11" r:id="rId37" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_HOAUC-2685Y-112CNG1SNA01_C350303.html" xr:uid="{1BB65DA6-8F70-45D7-ADC9-31E73153A346}"/>
     <hyperlink ref="J36" r:id="rId38" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-Female-header-1-8P-2-54mm-Straight-line_C124416.html" xr:uid="{120D961E-1337-4A68-B5D8-78D5C809202E}"/>
@@ -4480,11 +4518,15 @@
     <hyperlink ref="J58" r:id="rId49" display="https://lcsc.com/product-detail/Shunts-Jumpers_BOOMELE-Boom-Precision-Elec-C100114_C100114.html" xr:uid="{3B986909-AB08-4903-9FC2-4ED0C15097DF}"/>
     <hyperlink ref="J25" r:id="rId50" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_Ckmtw-Shenzhen-Cankemeng-Headers-Pins-2-5P-2-54mm-Straight-line_C124387.html" xr:uid="{C8C02C2D-AB0B-49A6-8D2F-B364B37C3B93}"/>
     <hyperlink ref="I36" r:id="rId51" display="https://lcsc.com/product-detail/Pin-Header-Female-Header_BOOMELE-Boom-Precision-Elec-2-54mm-1-8P-Straight-Female-header_C27438.html" xr:uid="{8CFF675A-5B77-4C96-937A-D09D917A58EF}"/>
-    <hyperlink ref="J59" r:id="rId52" display="https://lcsc.com/product-detail/Precision-Potentiometer_BOCHEN-Chengdu-Guosheng-Tech-3266W-1-203_C124983.html" xr:uid="{CA13AF68-61FC-4064-89E2-34536F2B755A}"/>
-    <hyperlink ref="I59" r:id="rId53" display="https://lcsc.com/product-detail/Precision-Potentiometer_BOCHEN-Chengdu-Guosheng-Tech-3266W-1-203_C124983.html" xr:uid="{405AF7DC-500C-411C-94B4-9E4DA3BD5513}"/>
+    <hyperlink ref="J59" r:id="rId52" display="https://lcsc.com/product-detail/MOSFET_SINO-IC-SE4942B_C238652.html" xr:uid="{D06F88E7-D04C-461E-A9A7-35710799C6AB}"/>
+    <hyperlink ref="I59" r:id="rId53" display="https://lcsc.com/product-detail/MOSFET_SINO-IC-SE4942B_C238652.html" xr:uid="{A2E45643-8A56-438E-B25E-F56AE9FABC69}"/>
+    <hyperlink ref="J50" r:id="rId54" display="https://lcsc.com/product-detail/MOSFET_Shikues-IRLML2402_C475705.html" xr:uid="{91DB62E6-688E-4E69-BC8A-19787E5FD2DA}"/>
+    <hyperlink ref="I50" r:id="rId55" display="https://lcsc.com/product-detail/MOSFET_Shikues-IRLML2402_C475705.html" xr:uid="{E02A3111-64D5-4374-828F-EC596C220973}"/>
+    <hyperlink ref="J60" r:id="rId56" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJ-PA3F2000V_C254528.html" xr:uid="{CC0F8C96-DF92-411F-B776-7349513749E6}"/>
+    <hyperlink ref="I60" r:id="rId57" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJ-PA3F2000V_C254528.html" xr:uid="{EC34942D-C732-40EA-AD03-941572EC7AD9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId54"/>
+  <pageSetup orientation="portrait" r:id="rId58"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changed voltage divider for THC input
</commit_message>
<xml_diff>
--- a/Hardware/Dring Heath Small/BOM LCSC.xlsx
+++ b/Hardware/Dring Heath Small/BOM LCSC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Hardware\Dring Heath Small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7E5E559-31CB-4F1E-B85B-ECDF52545A24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74156598-778A-47F3-8618-5B4EF7B2596B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30825" yWindow="1200" windowWidth="20280" windowHeight="12885" activeTab="1" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="314">
   <si>
     <t>Package</t>
   </si>
@@ -985,6 +985,15 @@
   </si>
   <si>
     <t>C254528</t>
+  </si>
+  <si>
+    <t>22nf ceramic Cap</t>
+  </si>
+  <si>
+    <t>CC0603JRX7R8BB223</t>
+  </si>
+  <si>
+    <t>C327290</t>
   </si>
 </sst>
 </file>
@@ -2743,10 +2752,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CF0671-FE26-4F07-89AC-F4C1AA2B534B}">
-  <dimension ref="A2:N60"/>
+  <dimension ref="A2:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4463,6 +4472,26 @@
       </c>
       <c r="J60" s="11" t="s">
         <v>309</v>
+      </c>
+      <c r="K60">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12">
+      <c r="C61" t="s">
+        <v>307</v>
+      </c>
+      <c r="E61" t="s">
+        <v>311</v>
+      </c>
+      <c r="I61" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="J61" s="11" t="s">
+        <v>312</v>
+      </c>
+      <c r="K61">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -4524,9 +4553,11 @@
     <hyperlink ref="I50" r:id="rId55" display="https://lcsc.com/product-detail/MOSFET_Shikues-IRLML2402_C475705.html" xr:uid="{E02A3111-64D5-4374-828F-EC596C220973}"/>
     <hyperlink ref="J60" r:id="rId56" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJ-PA3F2000V_C254528.html" xr:uid="{CC0F8C96-DF92-411F-B776-7349513749E6}"/>
     <hyperlink ref="I60" r:id="rId57" display="https://lcsc.com/product-detail/Chip-Resistor-Surface-Mount_PANASONIC-ERJ-PA3F2000V_C254528.html" xr:uid="{EC34942D-C732-40EA-AD03-941572EC7AD9}"/>
+    <hyperlink ref="J61" r:id="rId58" display="https://lcsc.com/product-detail/Others_YAGEO-CC0603JRX7R8BB223_C327290.html" xr:uid="{09FFC90C-A61F-41A5-BA2C-DF267E89FE93}"/>
+    <hyperlink ref="I61" r:id="rId59" display="https://lcsc.com/product-detail/Others_YAGEO-CC0603JRX7R8BB223_C327290.html" xr:uid="{1A88698B-F687-40CF-8951-D318782B0AEF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId58"/>
+  <pageSetup orientation="portrait" r:id="rId60"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added external A/D ADS1115
</commit_message>
<xml_diff>
--- a/Hardware/Dring Heath Small/BOM LCSC.xlsx
+++ b/Hardware/Dring Heath Small/BOM LCSC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Hardware\Dring Heath Small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74156598-778A-47F3-8618-5B4EF7B2596B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B9FA83-EE3D-4C57-A5BD-2D638BF882E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30825" yWindow="1200" windowWidth="20280" windowHeight="12885" activeTab="1" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
+    <workbookView xWindow="28680" yWindow="330" windowWidth="25440" windowHeight="15990" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="330">
   <si>
     <t>Package</t>
   </si>
@@ -780,12 +780,6 @@
     <t>Plasma V+</t>
   </si>
   <si>
-    <t>To Ready 8</t>
-  </si>
-  <si>
-    <t>To Ready 7</t>
-  </si>
-  <si>
     <t>To Ready</t>
   </si>
   <si>
@@ -994,6 +988,60 @@
   </si>
   <si>
     <t>C327290</t>
+  </si>
+  <si>
+    <t>Ready</t>
+  </si>
+  <si>
+    <t>TIO14</t>
+  </si>
+  <si>
+    <t>TIO12</t>
+  </si>
+  <si>
+    <t>Handover 9</t>
+  </si>
+  <si>
+    <t>Handover 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torch Module </t>
+  </si>
+  <si>
+    <t>Gnd</t>
+  </si>
+  <si>
+    <t>TIO25</t>
+  </si>
+  <si>
+    <t>TIO26</t>
+  </si>
+  <si>
+    <t>TIO27</t>
+  </si>
+  <si>
+    <t>TI017</t>
+  </si>
+  <si>
+    <t>I2S</t>
+  </si>
+  <si>
+    <t>12S</t>
+  </si>
+  <si>
+    <t>PLASMA VOLTAGE</t>
+  </si>
+  <si>
+    <t>ZLIM</t>
+  </si>
+  <si>
+    <t>ALIM</t>
+  </si>
+  <si>
+    <t>BLIM</t>
+  </si>
+  <si>
+    <t>CLIM</t>
   </si>
 </sst>
 </file>
@@ -1113,7 +1161,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1138,6 +1186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1473,20 +1522,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823C39F3-7594-4535-810B-0496FC455A11}">
-  <dimension ref="B1:O81"/>
+  <dimension ref="B1:O91"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="N74" sqref="N74"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.140625" customWidth="1"/>
+    <col min="2" max="2" width="57.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" customWidth="1"/>
@@ -1547,16 +1596,16 @@
         <v>215</v>
       </c>
       <c r="K4" s="15" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="L4" s="15" t="s">
         <v>27</v>
       </c>
       <c r="M4" s="15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="N4" s="15" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="O4" s="15"/>
     </row>
@@ -1648,13 +1697,13 @@
         <v>212</v>
       </c>
       <c r="C10" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="D10">
         <v>26</v>
       </c>
-      <c r="E10">
-        <v>21</v>
+      <c r="E10" s="18">
+        <v>12</v>
       </c>
       <c r="G10" t="s">
         <v>202</v>
@@ -1688,7 +1737,7 @@
         <v>206</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J11" s="16">
         <v>5</v>
@@ -1709,13 +1758,13 @@
     </row>
     <row r="12" spans="2:15">
       <c r="B12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C12" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E12">
         <v>33</v>
@@ -1727,7 +1776,7 @@
         <v>202</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J12" s="16">
         <v>6</v>
@@ -1773,13 +1822,13 @@
     </row>
     <row r="14" spans="2:15">
       <c r="B14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E14">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G14" t="s">
         <v>202</v>
@@ -1798,19 +1847,19 @@
     </row>
     <row r="15" spans="2:15">
       <c r="B15" t="s">
+        <v>250</v>
+      </c>
+      <c r="C15" t="s">
         <v>252</v>
       </c>
-      <c r="C15" t="s">
-        <v>254</v>
-      </c>
       <c r="D15" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E15">
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I15" s="15"/>
       <c r="J15" s="16"/>
@@ -1824,10 +1873,10 @@
     </row>
     <row r="16" spans="2:15">
       <c r="B16" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J16" s="16">
         <v>1</v>
@@ -1844,7 +1893,7 @@
     </row>
     <row r="17" spans="2:15">
       <c r="B17" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="I17" s="15"/>
       <c r="J17" s="16">
@@ -1880,7 +1929,7 @@
     </row>
     <row r="19" spans="2:15">
       <c r="B19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E19">
         <v>32</v>
@@ -1904,7 +1953,7 @@
     </row>
     <row r="20" spans="2:15">
       <c r="B20" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E20">
         <v>19</v>
@@ -1924,7 +1973,7 @@
     </row>
     <row r="21" spans="2:15">
       <c r="B21" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I21" s="15"/>
       <c r="J21" s="16">
@@ -1956,16 +2005,16 @@
     </row>
     <row r="23" spans="2:15">
       <c r="B23" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J23" s="16">
         <v>8</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="L23" s="15"/>
       <c r="M23" s="16">
@@ -1985,7 +2034,7 @@
     </row>
     <row r="25" spans="2:15">
       <c r="I25" s="15" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J25" s="16">
         <v>1</v>
@@ -2029,15 +2078,15 @@
       <c r="J28" s="16">
         <v>4</v>
       </c>
-      <c r="K28" s="15">
-        <v>9</v>
+      <c r="K28" s="15" t="s">
+        <v>315</v>
       </c>
       <c r="L28" s="15"/>
       <c r="M28" s="15" t="s">
         <v>228</v>
       </c>
       <c r="N28" s="15" t="s">
-        <v>229</v>
+        <v>314</v>
       </c>
       <c r="O28" s="15"/>
     </row>
@@ -2069,21 +2118,17 @@
     </row>
     <row r="31" spans="2:15">
       <c r="I31" s="15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J31" s="16">
         <v>7</v>
       </c>
-      <c r="K31" s="15" t="s">
-        <v>242</v>
-      </c>
+      <c r="K31" s="15"/>
       <c r="L31" s="15"/>
       <c r="M31" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="N31" s="15" t="s">
-        <v>233</v>
-      </c>
+      <c r="N31" s="15"/>
       <c r="O31" s="15"/>
     </row>
     <row r="32" spans="2:15">
@@ -2092,14 +2137,12 @@
         <v>8</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>243</v>
+        <v>312</v>
       </c>
       <c r="L32" s="15"/>
-      <c r="M32" s="15" t="s">
-        <v>232</v>
-      </c>
+      <c r="M32" s="15"/>
       <c r="N32" s="15" t="s">
-        <v>233</v>
+        <v>313</v>
       </c>
       <c r="O32" s="15"/>
     </row>
@@ -2108,15 +2151,15 @@
       <c r="J33" s="16">
         <v>9</v>
       </c>
-      <c r="K33" s="15">
-        <v>4</v>
+      <c r="K33" s="15" t="s">
+        <v>316</v>
       </c>
       <c r="L33" s="15"/>
       <c r="M33" s="15" t="s">
         <v>228</v>
       </c>
       <c r="N33" s="15" t="s">
-        <v>229</v>
+        <v>314</v>
       </c>
       <c r="O33" s="15"/>
     </row>
@@ -2131,7 +2174,7 @@
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
       <c r="N34" s="15" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="O34" s="15"/>
     </row>
@@ -2183,7 +2226,7 @@
     </row>
     <row r="39" spans="9:15">
       <c r="I39" s="15" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="J39" s="16">
         <v>1</v>
@@ -2202,7 +2245,7 @@
         <v>2</v>
       </c>
       <c r="K40" s="15" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="L40" s="15"/>
       <c r="M40" s="15"/>
@@ -2228,7 +2271,7 @@
         <v>4</v>
       </c>
       <c r="K42" s="15" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L42" s="15"/>
       <c r="M42" s="15"/>
@@ -2254,7 +2297,7 @@
         <v>6</v>
       </c>
       <c r="K44" s="15" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L44" s="15"/>
       <c r="M44" s="15"/>
@@ -2280,7 +2323,7 @@
         <v>8</v>
       </c>
       <c r="K46" s="15" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="L46" s="15"/>
       <c r="M46" s="15"/>
@@ -2293,7 +2336,7 @@
         <v>9</v>
       </c>
       <c r="K47" s="15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L47" s="15"/>
       <c r="M47" s="15"/>
@@ -2306,7 +2349,7 @@
         <v>10</v>
       </c>
       <c r="K48" s="15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L48" s="15"/>
       <c r="M48" s="15"/>
@@ -2324,7 +2367,7 @@
     </row>
     <row r="50" spans="9:15">
       <c r="I50" s="15" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J50" s="16">
         <v>1</v>
@@ -2343,10 +2386,10 @@
         <v>2</v>
       </c>
       <c r="K51" s="15" t="s">
+        <v>271</v>
+      </c>
+      <c r="L51" s="15" t="s">
         <v>273</v>
-      </c>
-      <c r="L51" s="15" t="s">
-        <v>275</v>
       </c>
       <c r="M51" s="15"/>
       <c r="N51" s="15"/>
@@ -2374,7 +2417,7 @@
         <v>195</v>
       </c>
       <c r="L53" s="15" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="M53" s="15"/>
       <c r="N53" s="15"/>
@@ -2383,10 +2426,10 @@
     <row r="54" spans="9:15">
       <c r="I54" s="15"/>
       <c r="J54" s="16" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K54" s="15" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
@@ -2404,7 +2447,7 @@
     </row>
     <row r="56" spans="9:15">
       <c r="I56" s="15" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J56" s="16">
         <v>1</v>
@@ -2436,7 +2479,7 @@
         <v>6</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L58" s="15"/>
       <c r="M58" s="15"/>
@@ -2449,7 +2492,7 @@
         <v>7</v>
       </c>
       <c r="K59" s="15" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
@@ -2480,13 +2523,13 @@
     </row>
     <row r="62" spans="9:15">
       <c r="I62" s="15" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="J62" s="16">
         <v>1</v>
       </c>
       <c r="K62" s="15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="L62" s="15"/>
       <c r="M62" s="15"/>
@@ -2499,7 +2542,7 @@
         <v>2</v>
       </c>
       <c r="K63" s="15" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L63" s="15"/>
       <c r="M63" s="15"/>
@@ -2512,7 +2555,7 @@
         <v>3</v>
       </c>
       <c r="K64" s="15" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="L64" s="15"/>
       <c r="M64" s="15"/>
@@ -2525,7 +2568,7 @@
         <v>4</v>
       </c>
       <c r="K65" s="15" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
@@ -2538,7 +2581,7 @@
         <v>5</v>
       </c>
       <c r="K66" s="15" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="L66" s="15"/>
       <c r="M66" s="15"/>
@@ -2551,7 +2594,7 @@
         <v>6</v>
       </c>
       <c r="K67" s="15" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L67" s="15"/>
       <c r="M67" s="15"/>
@@ -2564,7 +2607,7 @@
         <v>7</v>
       </c>
       <c r="K68" s="15" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="L68" s="15"/>
       <c r="M68" s="15"/>
@@ -2577,7 +2620,7 @@
         <v>8</v>
       </c>
       <c r="K69" s="15" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="L69" s="15"/>
       <c r="M69" s="15"/>
@@ -2595,7 +2638,7 @@
     </row>
     <row r="71" spans="9:15">
       <c r="I71" s="15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J71" s="16">
         <v>1</v>
@@ -2604,7 +2647,7 @@
         <v>21</v>
       </c>
       <c r="L71" s="15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="M71" s="15"/>
       <c r="N71" s="15"/>
@@ -2616,10 +2659,10 @@
         <v>2</v>
       </c>
       <c r="K72" s="15" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="L72" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="M72" s="15"/>
       <c r="N72" s="15"/>
@@ -2631,10 +2674,10 @@
         <v>3</v>
       </c>
       <c r="K73" s="15" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="L73" s="15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M73" s="15"/>
       <c r="N73" s="15"/>
@@ -2646,10 +2689,10 @@
         <v>4</v>
       </c>
       <c r="K74" s="15" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="L74" s="15" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M74" s="15"/>
       <c r="N74" s="15"/>
@@ -2661,10 +2704,10 @@
         <v>5</v>
       </c>
       <c r="K75" s="15" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="L75" s="15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M75" s="15"/>
       <c r="N75" s="15"/>
@@ -2676,10 +2719,10 @@
         <v>6</v>
       </c>
       <c r="K76" s="15" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="L76" s="15" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M76" s="15"/>
       <c r="N76" s="15"/>
@@ -2691,10 +2734,10 @@
         <v>8</v>
       </c>
       <c r="K77" s="15" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="L77" s="15" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="M77" s="15"/>
       <c r="N77" s="15"/>
@@ -2706,10 +2749,10 @@
         <v>9</v>
       </c>
       <c r="K78" s="15" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="L78" s="15" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="M78" s="15"/>
       <c r="N78" s="15"/>
@@ -2725,27 +2768,142 @@
       <c r="O79" s="15"/>
     </row>
     <row r="80" spans="9:15">
-      <c r="I80" s="15"/>
-      <c r="J80" s="16"/>
+      <c r="I80" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="J80" s="16">
+        <v>1</v>
+      </c>
       <c r="K80" s="15"/>
       <c r="L80" s="15"/>
       <c r="M80" s="15"/>
-      <c r="N80" s="15"/>
+      <c r="N80" s="15" t="s">
+        <v>318</v>
+      </c>
       <c r="O80" s="15"/>
     </row>
     <row r="81" spans="9:15">
       <c r="I81" s="15"/>
-      <c r="J81" s="16"/>
+      <c r="J81" s="16">
+        <v>2</v>
+      </c>
       <c r="K81" s="15"/>
       <c r="L81" s="15"/>
       <c r="M81" s="15"/>
-      <c r="N81" s="15"/>
+      <c r="N81" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="O81" s="15"/>
+    </row>
+    <row r="82" spans="9:15">
+      <c r="J82" s="17">
+        <v>3</v>
+      </c>
+      <c r="N82" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="83" spans="9:15">
+      <c r="J83" s="17">
+        <v>4</v>
+      </c>
+      <c r="K83" t="s">
+        <v>329</v>
+      </c>
+      <c r="N83" s="15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="84" spans="9:15">
+      <c r="J84" s="17">
+        <v>5</v>
+      </c>
+      <c r="K84" t="s">
+        <v>328</v>
+      </c>
+      <c r="N84" s="15" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="85" spans="9:15">
+      <c r="J85" s="17">
+        <v>6</v>
+      </c>
+      <c r="K85" t="s">
+        <v>327</v>
+      </c>
+      <c r="N85" s="15" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="86" spans="9:15">
+      <c r="J86" s="17">
+        <v>7</v>
+      </c>
+      <c r="K86" t="s">
+        <v>326</v>
+      </c>
+      <c r="N86" s="15" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="87" spans="9:15">
+      <c r="J87" s="17">
+        <v>8</v>
+      </c>
+      <c r="K87" t="s">
+        <v>325</v>
+      </c>
+      <c r="N87" s="15" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="88" spans="9:15">
+      <c r="J88" s="17">
+        <v>9</v>
+      </c>
+      <c r="K88" t="s">
+        <v>324</v>
+      </c>
+      <c r="N88" s="15" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="89" spans="9:15">
+      <c r="J89" s="17">
+        <v>10</v>
+      </c>
+      <c r="K89" t="s">
+        <v>323</v>
+      </c>
+      <c r="N89" s="15" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="90" spans="9:15">
+      <c r="J90" s="17">
+        <v>11</v>
+      </c>
+      <c r="K90" t="s">
+        <v>323</v>
+      </c>
+      <c r="N90" s="15" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="91" spans="9:15">
+      <c r="J91" s="17">
+        <v>12</v>
+      </c>
+      <c r="N91" s="15" t="s">
+        <v>282</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2754,7 +2912,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CF0671-FE26-4F07-89AC-F4C1AA2B534B}">
   <dimension ref="A2:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
@@ -4253,7 +4411,7 @@
         <v>1</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="F50" s="7" t="s">
         <v>4</v>
@@ -4265,10 +4423,10 @@
         <v>4</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J50" s="11" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K50">
         <v>20</v>
@@ -4445,16 +4603,16 @@
     </row>
     <row r="59" spans="1:12">
       <c r="C59" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="E59" t="s">
+        <v>299</v>
+      </c>
+      <c r="I59" s="11" t="s">
+        <v>301</v>
+      </c>
+      <c r="J59" s="11" t="s">
         <v>300</v>
-      </c>
-      <c r="E59" t="s">
-        <v>301</v>
-      </c>
-      <c r="I59" s="11" t="s">
-        <v>303</v>
-      </c>
-      <c r="J59" s="11" t="s">
-        <v>302</v>
       </c>
       <c r="K59">
         <v>20</v>
@@ -4462,16 +4620,16 @@
     </row>
     <row r="60" spans="1:12">
       <c r="C60" t="s">
+        <v>305</v>
+      </c>
+      <c r="E60" t="s">
+        <v>306</v>
+      </c>
+      <c r="I60" s="11" t="s">
+        <v>308</v>
+      </c>
+      <c r="J60" s="11" t="s">
         <v>307</v>
-      </c>
-      <c r="E60" t="s">
-        <v>308</v>
-      </c>
-      <c r="I60" s="11" t="s">
-        <v>310</v>
-      </c>
-      <c r="J60" s="11" t="s">
-        <v>309</v>
       </c>
       <c r="K60">
         <v>60</v>
@@ -4479,16 +4637,16 @@
     </row>
     <row r="61" spans="1:12">
       <c r="C61" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E61" t="s">
+        <v>309</v>
+      </c>
+      <c r="I61" s="11" t="s">
         <v>311</v>
       </c>
-      <c r="I61" s="11" t="s">
-        <v>313</v>
-      </c>
       <c r="J61" s="11" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="K61">
         <v>50</v>

</xml_diff>

<commit_message>
Torch1Module.sch alternate A/D input
</commit_message>
<xml_diff>
--- a/Hardware/Dring Heath Small/BOM LCSC.xlsx
+++ b/Hardware/Dring Heath Small/BOM LCSC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Hardware\Dring Heath Small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EEC42A-F49C-43EB-A095-2489623658A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD459AD1-9DED-4D30-9991-A583D8980F54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="330" windowWidth="25440" windowHeight="15990" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
+    <workbookView xWindow="28680" yWindow="330" windowWidth="25440" windowHeight="15990" activeTab="2" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="333">
   <si>
     <t>Package</t>
   </si>
@@ -1045,6 +1045,12 @@
   </si>
   <si>
     <t>I2S SDA</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>output</t>
   </si>
 </sst>
 </file>
@@ -1213,6 +1219,941 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Torch Module'!$B$2:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4FC6-4AE5-8B82-737048CABFE1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Torch Module'!$C$2:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.55900000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0589999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.73</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.91</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.09</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.4249999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4FC6-4AE5-8B82-737048CABFE1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="364548360"/>
+        <c:axId val="364550984"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="364548360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="364550984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="364550984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="364548360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -1313,6 +2254,47 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{134661DC-5044-4994-B15B-9069805E7E46}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1632,7 +2614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823C39F3-7594-4535-810B-0496FC455A11}">
   <dimension ref="B1:O91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
@@ -4833,9 +5815,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192ADD7D-D55E-4CB1-B608-DE63AF189E80}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -4848,8 +5832,90 @@
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3">
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>0.55900000000000005</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.0589999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4">
+        <v>1.5</v>
+      </c>
+      <c r="C4">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6">
+        <v>2.5</v>
+      </c>
+      <c r="C6">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>2.09</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8">
+        <v>3.5</v>
+      </c>
+      <c r="C8">
+        <v>2.2599999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>2.4249999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10">
+        <v>4.5</v>
+      </c>
+      <c r="C10">
+        <v>2.6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated torch module boards for external reset
</commit_message>
<xml_diff>
--- a/Hardware/Dring Heath Small/BOM LCSC.xlsx
+++ b/Hardware/Dring Heath Small/BOM LCSC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Plasma-Board\Hardware\Dring Heath Small\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD459AD1-9DED-4D30-9991-A583D8980F54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3574B72E-ED31-4201-8B71-0656729F8B50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="330" windowWidth="25440" windowHeight="15990" activeTab="2" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
+    <workbookView xWindow="28680" yWindow="330" windowWidth="25440" windowHeight="15990" xr2:uid="{3758BE0A-FED1-4CE6-972E-E965A802D2E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="2" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="342">
   <si>
     <t>Package</t>
   </si>
@@ -1005,9 +1005,6 @@
     <t>Handover 4</t>
   </si>
   <si>
-    <t xml:space="preserve">Torch Module </t>
-  </si>
-  <si>
     <t>Gnd</t>
   </si>
   <si>
@@ -1051,6 +1048,36 @@
   </si>
   <si>
     <t>output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THC ESP32 Module </t>
+  </si>
+  <si>
+    <t>A/D</t>
+  </si>
+  <si>
+    <t>J17</t>
+  </si>
+  <si>
+    <t>J18</t>
+  </si>
+  <si>
+    <t>RJ-7</t>
+  </si>
+  <si>
+    <t>RJ-8</t>
+  </si>
+  <si>
+    <t>RJ-3</t>
+  </si>
+  <si>
+    <t>RJ-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Could be jumpered </t>
+  </si>
+  <si>
+    <t>from ESP32 reset</t>
   </si>
 </sst>
 </file>
@@ -1100,7 +1127,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1116,6 +1143,36 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1170,7 +1227,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1188,23 +1245,109 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="8">
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2301,15 +2444,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{716ADE6A-35CE-4E4C-B219-B1B1F4F9A75F}" name="Table1" displayName="Table1" ref="I4:N78" totalsRowShown="0" headerRowCellStyle="Neutral" dataCellStyle="Neutral">
-  <autoFilter ref="I4:N78" xr:uid="{6121EDE4-EC13-44B8-ADB0-EBB42A872E42}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{716ADE6A-35CE-4E4C-B219-B1B1F4F9A75F}" name="Table1" displayName="Table1" ref="I4:N80" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowCellStyle="Neutral" dataCellStyle="Neutral">
+  <autoFilter ref="I4:N80" xr:uid="{6121EDE4-EC13-44B8-ADB0-EBB42A872E42}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{301FA929-2DD3-4704-BD79-3DF2D7C2A791}" name="Connectors" dataCellStyle="Neutral"/>
-    <tableColumn id="2" xr3:uid="{4AA82F2C-AE4C-41B2-8133-3C4AD65E22E5}" name="pins" dataDxfId="0" dataCellStyle="Neutral"/>
-    <tableColumn id="3" xr3:uid="{0AFD8132-CDB4-4DA3-AD7E-ECD258B75885}" name="Signal" dataCellStyle="Neutral"/>
-    <tableColumn id="4" xr3:uid="{C6F9D00A-3E2B-48F6-A3C8-25665E4C15D3}" name="Jumper" dataCellStyle="Neutral"/>
-    <tableColumn id="5" xr3:uid="{64BEA954-5FD2-4A22-B817-BA37E0208C5F}" name="GBRL" dataCellStyle="Neutral"/>
-    <tableColumn id="6" xr3:uid="{607FAAB1-E8A3-40CB-B205-7E92FF82AA41}" name="TCH" dataCellStyle="Neutral"/>
+    <tableColumn id="1" xr3:uid="{301FA929-2DD3-4704-BD79-3DF2D7C2A791}" name="Connectors" dataDxfId="7" dataCellStyle="Neutral"/>
+    <tableColumn id="2" xr3:uid="{4AA82F2C-AE4C-41B2-8133-3C4AD65E22E5}" name="pins" dataDxfId="6" dataCellStyle="Neutral"/>
+    <tableColumn id="3" xr3:uid="{0AFD8132-CDB4-4DA3-AD7E-ECD258B75885}" name="Signal" dataDxfId="5" dataCellStyle="Neutral"/>
+    <tableColumn id="4" xr3:uid="{C6F9D00A-3E2B-48F6-A3C8-25665E4C15D3}" name="Jumper" dataDxfId="4" dataCellStyle="Neutral"/>
+    <tableColumn id="5" xr3:uid="{64BEA954-5FD2-4A22-B817-BA37E0208C5F}" name="GBRL" dataDxfId="3" dataCellStyle="Neutral"/>
+    <tableColumn id="6" xr3:uid="{607FAAB1-E8A3-40CB-B205-7E92FF82AA41}" name="TCH" dataDxfId="2" dataCellStyle="Neutral"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2612,10 +2755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823C39F3-7594-4535-810B-0496FC455A11}">
-  <dimension ref="B1:O91"/>
+  <dimension ref="B1:O96"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="L82" sqref="L82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2629,7 +2772,7 @@
     <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.5703125" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11" style="17" customWidth="1"/>
+    <col min="10" max="10" width="11" style="15" customWidth="1"/>
     <col min="11" max="11" width="11.7109375" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
     <col min="13" max="13" width="13.7109375" customWidth="1"/>
@@ -2637,31 +2780,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
     </row>
     <row r="2" spans="2:15">
-      <c r="I2" s="15"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
     </row>
     <row r="3" spans="2:15">
-      <c r="I3" s="15"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
@@ -2679,64 +2822,64 @@
       <c r="G4" t="s">
         <v>201</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="K4" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="17" t="s">
         <v>260</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="O4" s="15"/>
+      <c r="O4" s="17"/>
     </row>
     <row r="5" spans="2:15">
-      <c r="I5" s="15"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="15"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
     </row>
     <row r="6" spans="2:15">
       <c r="B6" t="s">
         <v>193</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="19" t="s">
         <v>214</v>
       </c>
-      <c r="J6" s="16"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="15"/>
-      <c r="O6" s="15"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="17"/>
     </row>
     <row r="7" spans="2:15">
       <c r="B7" t="s">
         <v>194</v>
       </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="16">
+      <c r="I7" s="19"/>
+      <c r="J7" s="20">
         <v>1</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="17"/>
     </row>
     <row r="8" spans="2:15">
       <c r="B8" t="s">
@@ -2754,33 +2897,33 @@
       <c r="H8" t="s">
         <v>211</v>
       </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="16">
+      <c r="I8" s="19"/>
+      <c r="J8" s="20">
         <v>2</v>
       </c>
-      <c r="K8" s="15" t="s">
+      <c r="K8" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="15"/>
-      <c r="O8" s="15"/>
+      <c r="L8" s="19"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
+      <c r="O8" s="17"/>
     </row>
     <row r="9" spans="2:15">
       <c r="B9" t="s">
         <v>198</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16">
+      <c r="I9" s="19"/>
+      <c r="J9" s="20">
         <v>3</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="19" t="s">
         <v>217</v>
       </c>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
+      <c r="L9" s="19"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
+      <c r="O9" s="17"/>
     </row>
     <row r="10" spans="2:15">
       <c r="B10" t="s">
@@ -2792,23 +2935,23 @@
       <c r="D10">
         <v>26</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="16">
         <v>12</v>
       </c>
       <c r="G10" t="s">
         <v>202</v>
       </c>
-      <c r="I10" s="15"/>
-      <c r="J10" s="16">
-        <v>4</v>
-      </c>
-      <c r="K10" s="15" t="s">
+      <c r="I10" s="19"/>
+      <c r="J10" s="20">
+        <v>4</v>
+      </c>
+      <c r="K10" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="17"/>
     </row>
     <row r="11" spans="2:15">
       <c r="B11" t="s">
@@ -2826,25 +2969,25 @@
       <c r="H11" t="s">
         <v>206</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="J11" s="16">
+      <c r="J11" s="20">
         <v>5</v>
       </c>
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="19" t="s">
         <v>199</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="M11" s="15" t="s">
+      <c r="M11" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="N11" s="15" t="s">
+      <c r="N11" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="O11" s="15"/>
+      <c r="O11" s="17"/>
     </row>
     <row r="12" spans="2:15">
       <c r="B12" t="s">
@@ -2865,25 +3008,25 @@
       <c r="G12" t="s">
         <v>202</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="J12" s="16">
+      <c r="J12" s="20">
         <v>6</v>
       </c>
-      <c r="K12" s="15" t="s">
+      <c r="K12" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="19" t="s">
         <v>221</v>
       </c>
-      <c r="M12" s="15" t="s">
+      <c r="M12" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="N12" s="15" t="s">
+      <c r="N12" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="O12" s="15"/>
+      <c r="O12" s="17"/>
     </row>
     <row r="13" spans="2:15">
       <c r="B13" t="s">
@@ -2898,17 +3041,17 @@
       <c r="H13" t="s">
         <v>208</v>
       </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="16">
+      <c r="I13" s="19"/>
+      <c r="J13" s="20">
         <v>7</v>
       </c>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15" t="s">
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="O13" s="15"/>
+      <c r="O13" s="17"/>
     </row>
     <row r="14" spans="2:15">
       <c r="B14" t="s">
@@ -2923,17 +3066,17 @@
       <c r="G14" t="s">
         <v>202</v>
       </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="16">
+      <c r="I14" s="19"/>
+      <c r="J14" s="20">
         <v>8</v>
       </c>
-      <c r="K14" s="15" t="s">
+      <c r="K14" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="17"/>
     </row>
     <row r="15" spans="2:15">
       <c r="B15" t="s">
@@ -2951,71 +3094,71 @@
       <c r="F15" t="s">
         <v>254</v>
       </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15" t="s">
+      <c r="I15" s="19"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+      <c r="M15" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="17"/>
     </row>
     <row r="16" spans="2:15">
       <c r="B16" t="s">
         <v>275</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="19" t="s">
         <v>278</v>
       </c>
-      <c r="J16" s="16">
+      <c r="J16" s="20">
         <v>1</v>
       </c>
-      <c r="K16" s="15" t="s">
+      <c r="K16" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="L16" s="15"/>
-      <c r="M16" s="16">
+      <c r="L16" s="19"/>
+      <c r="M16" s="20">
         <v>3</v>
       </c>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
+      <c r="N16" s="19"/>
+      <c r="O16" s="17"/>
     </row>
     <row r="17" spans="2:15">
       <c r="B17" t="s">
         <v>255</v>
       </c>
-      <c r="I17" s="15"/>
-      <c r="J17" s="16">
+      <c r="I17" s="19"/>
+      <c r="J17" s="20">
         <v>2</v>
       </c>
-      <c r="K17" s="15" t="s">
+      <c r="K17" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="L17" s="15"/>
-      <c r="M17" s="16">
-        <v>4</v>
-      </c>
-      <c r="N17" s="15"/>
-      <c r="O17" s="15"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="20">
+        <v>4</v>
+      </c>
+      <c r="N17" s="19"/>
+      <c r="O17" s="17"/>
     </row>
     <row r="18" spans="2:15">
       <c r="B18" t="s">
         <v>203</v>
       </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="16">
+      <c r="I18" s="19"/>
+      <c r="J18" s="20">
         <v>3</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="L18" s="15"/>
-      <c r="M18" s="16">
+      <c r="L18" s="19"/>
+      <c r="M18" s="20">
         <v>6</v>
       </c>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="17"/>
     </row>
     <row r="19" spans="2:15">
       <c r="B19" t="s">
@@ -3027,19 +3170,19 @@
       <c r="G19" t="s">
         <v>207</v>
       </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="16">
-        <v>4</v>
-      </c>
-      <c r="K19" s="15" t="s">
+      <c r="I19" s="19"/>
+      <c r="J19" s="20">
+        <v>4</v>
+      </c>
+      <c r="K19" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="L19" s="15"/>
-      <c r="M19" s="16">
+      <c r="L19" s="19"/>
+      <c r="M19" s="20">
         <v>5</v>
       </c>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
+      <c r="N19" s="19"/>
+      <c r="O19" s="17"/>
     </row>
     <row r="20" spans="2:15">
       <c r="B20" t="s">
@@ -3051,944 +3194,1019 @@
       <c r="G20" t="s">
         <v>207</v>
       </c>
-      <c r="I20" s="15"/>
-      <c r="J20" s="16">
+      <c r="I20" s="19"/>
+      <c r="J20" s="20">
         <v>5</v>
       </c>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="20"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="17"/>
     </row>
     <row r="21" spans="2:15">
       <c r="B21" t="s">
         <v>258</v>
       </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="16">
+      <c r="I21" s="19"/>
+      <c r="J21" s="20">
         <v>6</v>
       </c>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
+      <c r="K21" s="19"/>
+      <c r="L21" s="19"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="19"/>
+      <c r="O21" s="17"/>
     </row>
     <row r="22" spans="2:15">
       <c r="B22" t="s">
         <v>194</v>
       </c>
-      <c r="I22" s="15"/>
-      <c r="J22" s="16">
+      <c r="I22" s="19"/>
+      <c r="J22" s="20">
         <v>7</v>
       </c>
-      <c r="K22" s="15" t="s">
+      <c r="K22" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="L22" s="15"/>
-      <c r="M22" s="16">
+      <c r="L22" s="19"/>
+      <c r="M22" s="20">
         <v>14</v>
       </c>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
+      <c r="N22" s="19"/>
+      <c r="O22" s="17"/>
     </row>
     <row r="23" spans="2:15">
       <c r="B23" t="s">
         <v>276</v>
       </c>
-      <c r="I23" s="15" t="s">
+      <c r="I23" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="J23" s="16">
+      <c r="J23" s="20">
         <v>8</v>
       </c>
-      <c r="K23" s="15" t="s">
+      <c r="K23" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="L23" s="15"/>
-      <c r="M23" s="16">
+      <c r="L23" s="19"/>
+      <c r="M23" s="20">
         <v>15</v>
       </c>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="17"/>
     </row>
     <row r="24" spans="2:15">
-      <c r="I24" s="15"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="17"/>
     </row>
     <row r="25" spans="2:15">
-      <c r="I25" s="15" t="s">
+      <c r="I25" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="J25" s="16">
+      <c r="J25" s="20">
         <v>1</v>
       </c>
-      <c r="K25" s="15" t="s">
+      <c r="K25" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+      <c r="N25" s="19"/>
+      <c r="O25" s="17"/>
     </row>
     <row r="26" spans="2:15">
-      <c r="I26" s="15"/>
-      <c r="J26" s="16">
+      <c r="I26" s="19"/>
+      <c r="J26" s="20">
         <v>2</v>
       </c>
-      <c r="K26" s="15" t="s">
+      <c r="K26" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="L26" s="15"/>
-      <c r="M26" s="15"/>
-      <c r="N26" s="15"/>
-      <c r="O26" s="15"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="17"/>
     </row>
     <row r="27" spans="2:15">
-      <c r="I27" s="15"/>
-      <c r="J27" s="16">
+      <c r="I27" s="19"/>
+      <c r="J27" s="20">
         <v>3</v>
       </c>
-      <c r="K27" s="15" t="s">
+      <c r="K27" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="17"/>
     </row>
     <row r="28" spans="2:15">
-      <c r="I28" s="15"/>
-      <c r="J28" s="16">
-        <v>4</v>
-      </c>
-      <c r="K28" s="15" t="s">
+      <c r="I28" s="19"/>
+      <c r="J28" s="20">
+        <v>4</v>
+      </c>
+      <c r="K28" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15" t="s">
+      <c r="L28" s="19"/>
+      <c r="M28" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="N28" s="15" t="s">
+      <c r="N28" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="O28" s="15"/>
+      <c r="O28" s="17"/>
     </row>
     <row r="29" spans="2:15">
-      <c r="I29" s="15"/>
-      <c r="J29" s="16">
+      <c r="I29" s="19"/>
+      <c r="J29" s="20">
         <v>5</v>
       </c>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15" t="s">
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19" t="s">
         <v>230</v>
       </c>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="17"/>
     </row>
     <row r="30" spans="2:15">
-      <c r="I30" s="15"/>
-      <c r="J30" s="16">
+      <c r="I30" s="19"/>
+      <c r="J30" s="20">
         <v>6</v>
       </c>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15" t="s">
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="17"/>
     </row>
     <row r="31" spans="2:15">
-      <c r="I31" s="15" t="s">
+      <c r="I31" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="J31" s="16">
+      <c r="J31" s="20">
         <v>7</v>
       </c>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15" t="s">
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="17"/>
     </row>
     <row r="32" spans="2:15">
-      <c r="I32" s="15"/>
-      <c r="J32" s="16">
+      <c r="I32" s="19"/>
+      <c r="J32" s="20">
         <v>8</v>
       </c>
-      <c r="K32" s="15" t="s">
+      <c r="K32" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15" t="s">
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="O32" s="15"/>
+      <c r="O32" s="17"/>
     </row>
     <row r="33" spans="9:15">
-      <c r="I33" s="15"/>
-      <c r="J33" s="16">
+      <c r="I33" s="19"/>
+      <c r="J33" s="20">
         <v>9</v>
       </c>
-      <c r="K33" s="15" t="s">
+      <c r="K33" s="19" t="s">
         <v>316</v>
       </c>
-      <c r="L33" s="15"/>
-      <c r="M33" s="15" t="s">
+      <c r="L33" s="19"/>
+      <c r="M33" s="19" t="s">
         <v>228</v>
       </c>
-      <c r="N33" s="15" t="s">
+      <c r="N33" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="O33" s="15"/>
+      <c r="O33" s="17"/>
     </row>
     <row r="34" spans="9:15">
-      <c r="I34" s="15"/>
-      <c r="J34" s="16">
+      <c r="I34" s="19"/>
+      <c r="J34" s="20">
         <v>10</v>
       </c>
-      <c r="K34" s="15" t="s">
+      <c r="K34" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15" t="s">
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19" t="s">
         <v>277</v>
       </c>
-      <c r="O34" s="15"/>
+      <c r="O34" s="17"/>
     </row>
     <row r="35" spans="9:15">
-      <c r="I35" s="15"/>
-      <c r="J35" s="16">
+      <c r="I35" s="19"/>
+      <c r="J35" s="20">
         <v>11</v>
       </c>
-      <c r="K35" s="15" t="s">
+      <c r="K35" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15" t="s">
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="O35" s="15"/>
+      <c r="O35" s="17"/>
     </row>
     <row r="36" spans="9:15">
-      <c r="I36" s="15"/>
-      <c r="J36" s="16">
+      <c r="I36" s="19"/>
+      <c r="J36" s="20">
         <v>12</v>
       </c>
-      <c r="K36" s="15" t="s">
+      <c r="K36" s="19" t="s">
         <v>216</v>
       </c>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="17"/>
     </row>
     <row r="37" spans="9:15">
-      <c r="I37" s="15"/>
-      <c r="J37" s="16"/>
-      <c r="K37" s="15"/>
-      <c r="L37" s="15"/>
-      <c r="M37" s="15"/>
-      <c r="N37" s="15"/>
-      <c r="O37" s="15"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="18"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
     </row>
     <row r="38" spans="9:15">
-      <c r="I38" s="15"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="18"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
     </row>
     <row r="39" spans="9:15">
-      <c r="I39" s="15" t="s">
+      <c r="I39" s="21" t="s">
         <v>268</v>
       </c>
-      <c r="J39" s="16">
+      <c r="J39" s="22">
         <v>1</v>
       </c>
-      <c r="K39" s="15" t="s">
+      <c r="K39" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="L39" s="15"/>
-      <c r="M39" s="15"/>
-      <c r="N39" s="15"/>
-      <c r="O39" s="15"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="17"/>
     </row>
     <row r="40" spans="9:15">
-      <c r="I40" s="15"/>
-      <c r="J40" s="16">
+      <c r="I40" s="21"/>
+      <c r="J40" s="22">
         <v>2</v>
       </c>
-      <c r="K40" s="15" t="s">
+      <c r="K40" s="21" t="s">
         <v>263</v>
       </c>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="17"/>
     </row>
     <row r="41" spans="9:15">
-      <c r="I41" s="15"/>
-      <c r="J41" s="16">
+      <c r="I41" s="21"/>
+      <c r="J41" s="22">
         <v>3</v>
       </c>
-      <c r="K41" s="15" t="s">
+      <c r="K41" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="17"/>
     </row>
     <row r="42" spans="9:15">
-      <c r="I42" s="15"/>
-      <c r="J42" s="16">
-        <v>4</v>
-      </c>
-      <c r="K42" s="15" t="s">
+      <c r="I42" s="21"/>
+      <c r="J42" s="22">
+        <v>4</v>
+      </c>
+      <c r="K42" s="21" t="s">
         <v>264</v>
       </c>
-      <c r="L42" s="15"/>
-      <c r="M42" s="15"/>
-      <c r="N42" s="15"/>
-      <c r="O42" s="15"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="17"/>
     </row>
     <row r="43" spans="9:15">
-      <c r="I43" s="15"/>
-      <c r="J43" s="16">
+      <c r="I43" s="21"/>
+      <c r="J43" s="22">
         <v>5</v>
       </c>
-      <c r="K43" s="15" t="s">
+      <c r="K43" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="17"/>
     </row>
     <row r="44" spans="9:15">
-      <c r="I44" s="15"/>
-      <c r="J44" s="16">
+      <c r="I44" s="21"/>
+      <c r="J44" s="22">
         <v>6</v>
       </c>
-      <c r="K44" s="15" t="s">
+      <c r="K44" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="21"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="17"/>
     </row>
     <row r="45" spans="9:15">
-      <c r="I45" s="15"/>
-      <c r="J45" s="16">
+      <c r="I45" s="21"/>
+      <c r="J45" s="22">
         <v>7</v>
       </c>
-      <c r="K45" s="15" t="s">
+      <c r="K45" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="L45" s="15"/>
-      <c r="M45" s="15"/>
-      <c r="N45" s="15"/>
-      <c r="O45" s="15"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="17"/>
     </row>
     <row r="46" spans="9:15">
-      <c r="I46" s="15"/>
-      <c r="J46" s="16">
+      <c r="I46" s="21"/>
+      <c r="J46" s="22">
         <v>8</v>
       </c>
-      <c r="K46" s="15" t="s">
+      <c r="K46" s="21" t="s">
         <v>266</v>
       </c>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="17"/>
     </row>
     <row r="47" spans="9:15">
-      <c r="I47" s="15"/>
-      <c r="J47" s="16">
+      <c r="I47" s="21"/>
+      <c r="J47" s="22">
         <v>9</v>
       </c>
-      <c r="K47" s="15" t="s">
+      <c r="K47" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="21"/>
+      <c r="N47" s="21"/>
+      <c r="O47" s="17"/>
     </row>
     <row r="48" spans="9:15">
-      <c r="I48" s="15"/>
-      <c r="J48" s="16">
+      <c r="I48" s="21"/>
+      <c r="J48" s="22">
         <v>10</v>
       </c>
-      <c r="K48" s="15" t="s">
+      <c r="K48" s="21" t="s">
         <v>262</v>
       </c>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="21"/>
+      <c r="N48" s="21"/>
+      <c r="O48" s="17"/>
     </row>
     <row r="49" spans="9:15">
-      <c r="I49" s="15"/>
-      <c r="J49" s="16"/>
-      <c r="K49" s="15"/>
-      <c r="L49" s="15"/>
-      <c r="M49" s="15"/>
-      <c r="N49" s="15"/>
-      <c r="O49" s="15"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="18"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
     </row>
     <row r="50" spans="9:15">
-      <c r="I50" s="15" t="s">
+      <c r="I50" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="J50" s="16">
+      <c r="J50" s="24">
         <v>1</v>
       </c>
-      <c r="K50" s="15" t="s">
+      <c r="K50" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="L50" s="15"/>
-      <c r="M50" s="15"/>
-      <c r="N50" s="15"/>
-      <c r="O50" s="15"/>
+      <c r="L50" s="23"/>
+      <c r="M50" s="23"/>
+      <c r="N50" s="23"/>
+      <c r="O50" s="17"/>
     </row>
     <row r="51" spans="9:15">
-      <c r="I51" s="15"/>
-      <c r="J51" s="16">
+      <c r="I51" s="23"/>
+      <c r="J51" s="24">
         <v>2</v>
       </c>
-      <c r="K51" s="15" t="s">
+      <c r="K51" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="L51" s="15" t="s">
+      <c r="L51" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="M51" s="15"/>
-      <c r="N51" s="15"/>
-      <c r="O51" s="15"/>
+      <c r="M51" s="23"/>
+      <c r="N51" s="23"/>
+      <c r="O51" s="17"/>
     </row>
     <row r="52" spans="9:15">
-      <c r="I52" s="15"/>
-      <c r="J52" s="16">
+      <c r="I52" s="23"/>
+      <c r="J52" s="24">
         <v>5</v>
       </c>
-      <c r="K52" s="15" t="s">
+      <c r="K52" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="L52" s="15"/>
-      <c r="M52" s="15"/>
-      <c r="N52" s="15"/>
-      <c r="O52" s="15"/>
+      <c r="L52" s="23"/>
+      <c r="M52" s="23"/>
+      <c r="N52" s="23"/>
+      <c r="O52" s="17"/>
     </row>
     <row r="53" spans="9:15">
-      <c r="I53" s="15"/>
-      <c r="J53" s="16">
+      <c r="I53" s="23"/>
+      <c r="J53" s="24">
         <v>6</v>
       </c>
-      <c r="K53" s="15" t="s">
+      <c r="K53" s="23" t="s">
         <v>195</v>
       </c>
-      <c r="L53" s="15" t="s">
+      <c r="L53" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
+      <c r="M53" s="23"/>
+      <c r="N53" s="23"/>
+      <c r="O53" s="17"/>
     </row>
     <row r="54" spans="9:15">
-      <c r="I54" s="15"/>
-      <c r="J54" s="16" t="s">
+      <c r="I54" s="23"/>
+      <c r="J54" s="24" t="s">
         <v>270</v>
       </c>
-      <c r="K54" s="15" t="s">
+      <c r="K54" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="L54" s="15"/>
-      <c r="M54" s="15"/>
-      <c r="N54" s="15"/>
-      <c r="O54" s="15"/>
+      <c r="L54" s="23"/>
+      <c r="M54" s="23"/>
+      <c r="N54" s="23"/>
+      <c r="O54" s="17"/>
     </row>
     <row r="55" spans="9:15">
-      <c r="I55" s="15"/>
-      <c r="J55" s="16"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="15"/>
-      <c r="M55" s="15"/>
-      <c r="N55" s="15"/>
-      <c r="O55" s="15"/>
+      <c r="I55" s="23"/>
+      <c r="J55" s="24"/>
+      <c r="K55" s="23"/>
+      <c r="L55" s="23"/>
+      <c r="M55" s="23"/>
+      <c r="N55" s="23"/>
+      <c r="O55" s="17"/>
     </row>
     <row r="56" spans="9:15">
-      <c r="I56" s="15" t="s">
+      <c r="I56" s="23" t="s">
         <v>267</v>
       </c>
-      <c r="J56" s="16">
+      <c r="J56" s="24">
         <v>1</v>
       </c>
-      <c r="K56" s="15" t="s">
+      <c r="K56" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="L56" s="15"/>
-      <c r="M56" s="15"/>
-      <c r="N56" s="15"/>
-      <c r="O56" s="15"/>
+      <c r="L56" s="23"/>
+      <c r="M56" s="23"/>
+      <c r="N56" s="23"/>
+      <c r="O56" s="17"/>
     </row>
     <row r="57" spans="9:15">
-      <c r="I57" s="15"/>
-      <c r="J57" s="16">
+      <c r="I57" s="23"/>
+      <c r="J57" s="24">
         <v>2</v>
       </c>
-      <c r="K57" s="15" t="s">
+      <c r="K57" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="L57" s="15"/>
-      <c r="M57" s="15"/>
-      <c r="N57" s="15"/>
-      <c r="O57" s="15"/>
+      <c r="L57" s="23"/>
+      <c r="M57" s="23"/>
+      <c r="N57" s="23"/>
+      <c r="O57" s="17"/>
     </row>
     <row r="58" spans="9:15">
-      <c r="I58" s="15"/>
-      <c r="J58" s="16">
+      <c r="I58" s="23"/>
+      <c r="J58" s="24">
         <v>6</v>
       </c>
-      <c r="K58" s="15" t="s">
+      <c r="K58" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="L58" s="15"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="15"/>
-      <c r="O58" s="15"/>
+      <c r="L58" s="23"/>
+      <c r="M58" s="23"/>
+      <c r="N58" s="23"/>
+      <c r="O58" s="17"/>
     </row>
     <row r="59" spans="9:15">
-      <c r="I59" s="15"/>
-      <c r="J59" s="16">
+      <c r="I59" s="23"/>
+      <c r="J59" s="24">
         <v>7</v>
       </c>
-      <c r="K59" s="15" t="s">
+      <c r="K59" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="L59" s="15"/>
-      <c r="M59" s="15"/>
-      <c r="N59" s="15"/>
-      <c r="O59" s="15"/>
+      <c r="L59" s="23"/>
+      <c r="M59" s="23"/>
+      <c r="N59" s="23"/>
+      <c r="O59" s="17"/>
     </row>
     <row r="60" spans="9:15">
-      <c r="I60" s="15"/>
-      <c r="J60" s="16">
+      <c r="I60" s="23"/>
+      <c r="J60" s="24">
         <v>12</v>
       </c>
-      <c r="K60" s="15" t="s">
+      <c r="K60" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="L60" s="15"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="15"/>
-      <c r="O60" s="15"/>
+      <c r="L60" s="23"/>
+      <c r="M60" s="23"/>
+      <c r="N60" s="23"/>
+      <c r="O60" s="17"/>
     </row>
     <row r="61" spans="9:15">
-      <c r="I61" s="15"/>
-      <c r="J61" s="16"/>
-      <c r="K61" s="15"/>
-      <c r="L61" s="15"/>
-      <c r="M61" s="15"/>
-      <c r="N61" s="15"/>
-      <c r="O61" s="15"/>
+      <c r="I61" s="17"/>
+      <c r="J61" s="18"/>
+      <c r="K61" s="17"/>
+      <c r="L61" s="17"/>
+      <c r="M61" s="17"/>
+      <c r="N61" s="17"/>
+      <c r="O61" s="17"/>
     </row>
     <row r="62" spans="9:15">
-      <c r="I62" s="15" t="s">
+      <c r="I62" s="25" t="s">
         <v>279</v>
       </c>
-      <c r="J62" s="16">
+      <c r="J62" s="26">
         <v>1</v>
       </c>
-      <c r="K62" s="15" t="s">
+      <c r="K62" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="L62" s="15"/>
-      <c r="M62" s="15"/>
-      <c r="N62" s="15"/>
-      <c r="O62" s="15"/>
+      <c r="L62" s="25"/>
+      <c r="M62" s="25"/>
+      <c r="N62" s="25"/>
+      <c r="O62" s="17"/>
     </row>
     <row r="63" spans="9:15">
-      <c r="I63" s="15"/>
-      <c r="J63" s="16">
+      <c r="I63" s="25"/>
+      <c r="J63" s="26">
         <v>2</v>
       </c>
-      <c r="K63" s="15" t="s">
+      <c r="K63" s="25" t="s">
         <v>283</v>
       </c>
-      <c r="L63" s="15"/>
-      <c r="M63" s="15"/>
-      <c r="N63" s="15"/>
-      <c r="O63" s="15"/>
+      <c r="L63" s="25"/>
+      <c r="M63" s="25"/>
+      <c r="N63" s="25"/>
+      <c r="O63" s="17"/>
     </row>
     <row r="64" spans="9:15">
-      <c r="I64" s="15"/>
-      <c r="J64" s="16">
+      <c r="I64" s="25"/>
+      <c r="J64" s="26">
         <v>3</v>
       </c>
-      <c r="K64" s="15" t="s">
+      <c r="K64" s="25" t="s">
         <v>284</v>
       </c>
-      <c r="L64" s="15"/>
-      <c r="M64" s="15"/>
-      <c r="N64" s="15"/>
-      <c r="O64" s="15"/>
+      <c r="L64" s="25"/>
+      <c r="M64" s="25"/>
+      <c r="N64" s="25"/>
+      <c r="O64" s="17"/>
     </row>
     <row r="65" spans="2:15">
       <c r="B65">
         <v>25</v>
       </c>
-      <c r="I65" s="15"/>
-      <c r="J65" s="16">
-        <v>4</v>
-      </c>
-      <c r="K65" s="15" t="s">
+      <c r="I65" s="25"/>
+      <c r="J65" s="26">
+        <v>4</v>
+      </c>
+      <c r="K65" s="25" t="s">
         <v>285</v>
       </c>
-      <c r="L65" s="15"/>
-      <c r="M65" s="15"/>
-      <c r="N65" s="15"/>
-      <c r="O65" s="15"/>
+      <c r="L65" s="25"/>
+      <c r="M65" s="25"/>
+      <c r="N65" s="25"/>
+      <c r="O65" s="17"/>
     </row>
     <row r="66" spans="2:15">
-      <c r="I66" s="15"/>
-      <c r="J66" s="16">
+      <c r="I66" s="25"/>
+      <c r="J66" s="26">
         <v>5</v>
       </c>
-      <c r="K66" s="15" t="s">
+      <c r="K66" s="25" t="s">
         <v>286</v>
       </c>
-      <c r="L66" s="15"/>
-      <c r="M66" s="15"/>
-      <c r="N66" s="15"/>
-      <c r="O66" s="15"/>
+      <c r="L66" s="25"/>
+      <c r="M66" s="25"/>
+      <c r="N66" s="25"/>
+      <c r="O66" s="17"/>
     </row>
     <row r="67" spans="2:15">
-      <c r="I67" s="15"/>
-      <c r="J67" s="16">
+      <c r="I67" s="25"/>
+      <c r="J67" s="26">
         <v>6</v>
       </c>
-      <c r="K67" s="15" t="s">
+      <c r="K67" s="25" t="s">
         <v>287</v>
       </c>
-      <c r="L67" s="15"/>
-      <c r="M67" s="15"/>
-      <c r="N67" s="15"/>
-      <c r="O67" s="15"/>
+      <c r="L67" s="25"/>
+      <c r="M67" s="25"/>
+      <c r="N67" s="25"/>
+      <c r="O67" s="17"/>
     </row>
     <row r="68" spans="2:15">
-      <c r="I68" s="15"/>
-      <c r="J68" s="16">
+      <c r="I68" s="25"/>
+      <c r="J68" s="26">
         <v>7</v>
       </c>
-      <c r="K68" s="15" t="s">
+      <c r="K68" s="25" t="s">
         <v>288</v>
       </c>
-      <c r="L68" s="15"/>
-      <c r="M68" s="15"/>
-      <c r="N68" s="15"/>
-      <c r="O68" s="15"/>
+      <c r="L68" s="25"/>
+      <c r="M68" s="25"/>
+      <c r="N68" s="25"/>
+      <c r="O68" s="17"/>
     </row>
     <row r="69" spans="2:15">
-      <c r="I69" s="15"/>
-      <c r="J69" s="16">
+      <c r="I69" s="25"/>
+      <c r="J69" s="26">
         <v>8</v>
       </c>
-      <c r="K69" s="15" t="s">
+      <c r="K69" s="25" t="s">
         <v>282</v>
       </c>
-      <c r="L69" s="15"/>
-      <c r="M69" s="15"/>
-      <c r="N69" s="15"/>
-      <c r="O69" s="15"/>
+      <c r="L69" s="25"/>
+      <c r="M69" s="25"/>
+      <c r="N69" s="25"/>
+      <c r="O69" s="17"/>
     </row>
     <row r="70" spans="2:15">
-      <c r="I70" s="15"/>
-      <c r="J70" s="16"/>
-      <c r="K70" s="15"/>
-      <c r="L70" s="15"/>
-      <c r="M70" s="15"/>
-      <c r="N70" s="15"/>
-      <c r="O70" s="15"/>
+      <c r="I70" s="25"/>
+      <c r="J70" s="26"/>
+      <c r="K70" s="25"/>
+      <c r="L70" s="25"/>
+      <c r="M70" s="25"/>
+      <c r="N70" s="25"/>
+      <c r="O70" s="17"/>
     </row>
     <row r="71" spans="2:15">
-      <c r="I71" s="15" t="s">
+      <c r="I71" s="25" t="s">
         <v>280</v>
       </c>
-      <c r="J71" s="16">
+      <c r="J71" s="26">
         <v>1</v>
       </c>
-      <c r="K71" s="15" t="s">
+      <c r="K71" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="L71" s="15" t="s">
+      <c r="L71" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="M71" s="15"/>
-      <c r="N71" s="15"/>
-      <c r="O71" s="15"/>
+      <c r="M71" s="25"/>
+      <c r="N71" s="25"/>
+      <c r="O71" s="17"/>
     </row>
     <row r="72" spans="2:15">
-      <c r="I72" s="15"/>
-      <c r="J72" s="16">
+      <c r="I72" s="25"/>
+      <c r="J72" s="26">
         <v>2</v>
       </c>
-      <c r="K72" s="15" t="s">
+      <c r="K72" s="25" t="s">
         <v>290</v>
       </c>
-      <c r="L72" s="15" t="s">
+      <c r="L72" s="25" t="s">
         <v>294</v>
       </c>
-      <c r="M72" s="15"/>
-      <c r="N72" s="15"/>
-      <c r="O72" s="15"/>
+      <c r="M72" s="25"/>
+      <c r="N72" s="25"/>
+      <c r="O72" s="17"/>
     </row>
     <row r="73" spans="2:15">
-      <c r="I73" s="15"/>
-      <c r="J73" s="16">
+      <c r="I73" s="25"/>
+      <c r="J73" s="26">
         <v>3</v>
       </c>
-      <c r="K73" s="15" t="s">
+      <c r="K73" s="25" t="s">
         <v>282</v>
       </c>
-      <c r="L73" s="15" t="s">
+      <c r="L73" s="25" t="s">
         <v>295</v>
       </c>
-      <c r="M73" s="15"/>
-      <c r="N73" s="15"/>
-      <c r="O73" s="15"/>
+      <c r="M73" s="25"/>
+      <c r="N73" s="25"/>
+      <c r="O73" s="17"/>
     </row>
     <row r="74" spans="2:15">
-      <c r="I74" s="15"/>
-      <c r="J74" s="16">
-        <v>4</v>
-      </c>
-      <c r="K74" s="15" t="s">
+      <c r="I74" s="25"/>
+      <c r="J74" s="26">
+        <v>4</v>
+      </c>
+      <c r="K74" s="25" t="s">
         <v>289</v>
       </c>
-      <c r="L74" s="15" t="s">
+      <c r="L74" s="25" t="s">
         <v>293</v>
       </c>
-      <c r="M74" s="15"/>
-      <c r="N74" s="15"/>
-      <c r="O74" s="15"/>
+      <c r="M74" s="25"/>
+      <c r="N74" s="25"/>
+      <c r="O74" s="17"/>
     </row>
     <row r="75" spans="2:15">
-      <c r="I75" s="15"/>
-      <c r="J75" s="16">
+      <c r="I75" s="25"/>
+      <c r="J75" s="26">
         <v>5</v>
       </c>
-      <c r="K75" s="15" t="s">
+      <c r="K75" s="25" t="s">
         <v>282</v>
       </c>
-      <c r="L75" s="15" t="s">
+      <c r="L75" s="25" t="s">
         <v>295</v>
       </c>
-      <c r="M75" s="15"/>
-      <c r="N75" s="15"/>
-      <c r="O75" s="15"/>
+      <c r="M75" s="25"/>
+      <c r="N75" s="25"/>
+      <c r="O75" s="17"/>
     </row>
     <row r="76" spans="2:15">
-      <c r="I76" s="15"/>
-      <c r="J76" s="16">
+      <c r="I76" s="25"/>
+      <c r="J76" s="26">
         <v>6</v>
       </c>
-      <c r="K76" s="15" t="s">
+      <c r="K76" s="25" t="s">
         <v>291</v>
       </c>
-      <c r="L76" s="15" t="s">
+      <c r="L76" s="25" t="s">
         <v>296</v>
       </c>
-      <c r="M76" s="15"/>
-      <c r="N76" s="15"/>
-      <c r="O76" s="15"/>
+      <c r="M76" s="25"/>
+      <c r="N76" s="25"/>
+      <c r="O76" s="17"/>
     </row>
     <row r="77" spans="2:15">
-      <c r="I77" s="15"/>
-      <c r="J77" s="16">
+      <c r="I77" s="25"/>
+      <c r="J77" s="26">
         <v>8</v>
       </c>
-      <c r="K77" s="15" t="s">
+      <c r="K77" s="25" t="s">
         <v>292</v>
       </c>
-      <c r="L77" s="15" t="s">
+      <c r="L77" s="25" t="s">
         <v>297</v>
       </c>
-      <c r="M77" s="15"/>
-      <c r="N77" s="15"/>
-      <c r="O77" s="15"/>
+      <c r="M77" s="25"/>
+      <c r="N77" s="25"/>
+      <c r="O77" s="17"/>
     </row>
     <row r="78" spans="2:15">
-      <c r="I78" s="15"/>
-      <c r="J78" s="16">
+      <c r="I78" s="25"/>
+      <c r="J78" s="26">
         <v>9</v>
       </c>
-      <c r="K78" s="15" t="s">
+      <c r="K78" s="25" t="s">
         <v>282</v>
       </c>
-      <c r="L78" s="15" t="s">
+      <c r="L78" s="25" t="s">
         <v>295</v>
       </c>
-      <c r="M78" s="15"/>
-      <c r="N78" s="15"/>
-      <c r="O78" s="15"/>
+      <c r="M78" s="25"/>
+      <c r="N78" s="25"/>
+      <c r="O78" s="17"/>
     </row>
     <row r="79" spans="2:15">
-      <c r="I79" s="15"/>
-      <c r="J79" s="16"/>
-      <c r="K79" s="15"/>
-      <c r="L79" s="15"/>
-      <c r="M79" s="15"/>
-      <c r="N79" s="15"/>
-      <c r="O79" s="15"/>
+      <c r="I79" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="J79" s="18">
+        <v>1</v>
+      </c>
+      <c r="K79" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="L79" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="M79" s="17"/>
+      <c r="N79" s="17"/>
+      <c r="O79" s="17"/>
     </row>
     <row r="80" spans="2:15">
-      <c r="I80" s="15" t="s">
+      <c r="I80" s="17"/>
+      <c r="J80" s="18">
+        <v>2</v>
+      </c>
+      <c r="K80" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="L80" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="M80" s="17"/>
+      <c r="N80" s="17"/>
+      <c r="O80" s="17"/>
+    </row>
+    <row r="81" spans="9:15">
+      <c r="I81" t="s">
+        <v>335</v>
+      </c>
+      <c r="J81" s="15">
+        <v>1</v>
+      </c>
+      <c r="K81" t="s">
+        <v>338</v>
+      </c>
+      <c r="O81" s="17"/>
+    </row>
+    <row r="82" spans="9:15">
+      <c r="J82" s="15">
+        <v>2</v>
+      </c>
+      <c r="K82" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="85" spans="9:15">
+      <c r="I85" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="J85" s="28">
+        <v>1</v>
+      </c>
+      <c r="K85" s="27"/>
+      <c r="L85" s="27"/>
+      <c r="M85" s="27"/>
+      <c r="N85" s="27" t="s">
         <v>317</v>
       </c>
-      <c r="J80" s="16">
-        <v>1</v>
-      </c>
-      <c r="K80" s="15"/>
-      <c r="L80" s="15"/>
-      <c r="M80" s="15"/>
-      <c r="N80" s="15" t="s">
+    </row>
+    <row r="86" spans="9:15">
+      <c r="I86" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="J86" s="28">
+        <v>2</v>
+      </c>
+      <c r="K86" s="27"/>
+      <c r="L86" s="27"/>
+      <c r="M86" s="27"/>
+      <c r="N86" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="9:15">
+      <c r="I87" s="29"/>
+      <c r="J87" s="30">
+        <v>3</v>
+      </c>
+      <c r="K87" s="29"/>
+      <c r="L87" s="29"/>
+      <c r="M87" s="29"/>
+      <c r="N87" s="29" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="88" spans="9:15">
+      <c r="I88" s="29"/>
+      <c r="J88" s="30">
+        <v>4</v>
+      </c>
+      <c r="K88" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="L88" s="29"/>
+      <c r="M88" s="29"/>
+      <c r="N88" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="89" spans="9:15">
+      <c r="I89" s="29"/>
+      <c r="J89" s="30">
+        <v>5</v>
+      </c>
+      <c r="K89" s="29" t="s">
+        <v>326</v>
+      </c>
+      <c r="L89" s="29"/>
+      <c r="M89" s="29"/>
+      <c r="N89" s="27" t="s">
         <v>318</v>
       </c>
-      <c r="O80" s="15"/>
-    </row>
-    <row r="81" spans="9:15">
-      <c r="I81" s="15"/>
-      <c r="J81" s="16">
-        <v>2</v>
-      </c>
-      <c r="K81" s="15"/>
-      <c r="L81" s="15"/>
-      <c r="M81" s="15"/>
-      <c r="N81" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="O81" s="15"/>
-    </row>
-    <row r="82" spans="9:15">
-      <c r="J82" s="17">
-        <v>3</v>
-      </c>
-      <c r="N82" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="83" spans="9:15">
-      <c r="J83" s="17">
-        <v>4</v>
-      </c>
-      <c r="K83" t="s">
+    </row>
+    <row r="90" spans="9:15">
+      <c r="I90" s="29"/>
+      <c r="J90" s="30">
+        <v>6</v>
+      </c>
+      <c r="K90" s="29" t="s">
+        <v>325</v>
+      </c>
+      <c r="L90" s="29"/>
+      <c r="M90" s="29"/>
+      <c r="N90" s="27" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="91" spans="9:15">
+      <c r="I91" s="29"/>
+      <c r="J91" s="30">
+        <v>7</v>
+      </c>
+      <c r="K91" s="29" t="s">
+        <v>324</v>
+      </c>
+      <c r="L91" s="29"/>
+      <c r="M91" s="29"/>
+      <c r="N91" s="27" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="92" spans="9:15">
+      <c r="I92" s="29"/>
+      <c r="J92" s="30">
+        <v>8</v>
+      </c>
+      <c r="K92" s="29" t="s">
+        <v>323</v>
+      </c>
+      <c r="L92" s="29"/>
+      <c r="M92" s="29"/>
+      <c r="N92" s="27" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="93" spans="9:15">
+      <c r="I93" s="29"/>
+      <c r="J93" s="30">
+        <v>9</v>
+      </c>
+      <c r="K93" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="L93" s="29"/>
+      <c r="M93" s="29"/>
+      <c r="N93" s="27" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="94" spans="9:15">
+      <c r="I94" s="29"/>
+      <c r="J94" s="30">
+        <v>10</v>
+      </c>
+      <c r="K94" s="29" t="s">
+        <v>329</v>
+      </c>
+      <c r="L94" s="29"/>
+      <c r="M94" s="29"/>
+      <c r="N94" s="27" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="95" spans="9:15">
+      <c r="I95" s="29"/>
+      <c r="J95" s="30">
+        <v>11</v>
+      </c>
+      <c r="K95" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="N83" s="15" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="84" spans="9:15">
-      <c r="J84" s="17">
-        <v>5</v>
-      </c>
-      <c r="K84" t="s">
-        <v>327</v>
-      </c>
-      <c r="N84" s="15" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="85" spans="9:15">
-      <c r="J85" s="17">
-        <v>6</v>
-      </c>
-      <c r="K85" t="s">
-        <v>326</v>
-      </c>
-      <c r="N85" s="15" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="86" spans="9:15">
-      <c r="J86" s="17">
-        <v>7</v>
-      </c>
-      <c r="K86" t="s">
-        <v>325</v>
-      </c>
-      <c r="N86" s="15" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="87" spans="9:15">
-      <c r="J87" s="17">
-        <v>8</v>
-      </c>
-      <c r="K87" t="s">
-        <v>324</v>
-      </c>
-      <c r="N87" s="15" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="88" spans="9:15">
-      <c r="J88" s="17">
-        <v>9</v>
-      </c>
-      <c r="K88" t="s">
-        <v>323</v>
-      </c>
-      <c r="N88" s="15" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="89" spans="9:15">
-      <c r="J89" s="17">
-        <v>10</v>
-      </c>
-      <c r="K89" t="s">
-        <v>330</v>
-      </c>
-      <c r="N89" s="15" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="90" spans="9:15">
-      <c r="J90" s="17">
-        <v>11</v>
-      </c>
-      <c r="K90" t="s">
-        <v>329</v>
-      </c>
-      <c r="N90" s="15" t="s">
+      <c r="L95" s="29"/>
+      <c r="M95" s="29"/>
+      <c r="N95" s="27" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="91" spans="9:15">
-      <c r="J91" s="17">
+    <row r="96" spans="9:15">
+      <c r="I96" s="29"/>
+      <c r="J96" s="30">
         <v>12</v>
       </c>
-      <c r="N91" s="15" t="s">
+      <c r="K96" s="29"/>
+      <c r="L96" s="29"/>
+      <c r="M96" s="29"/>
+      <c r="N96" s="27" t="s">
         <v>282</v>
       </c>
     </row>
@@ -5817,7 +6035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192ADD7D-D55E-4CB1-B608-DE63AF189E80}">
   <dimension ref="B1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C10"/>
     </sheetView>
   </sheetViews>
@@ -5835,10 +6053,10 @@
   <sheetData>
     <row r="1" spans="2:3">
       <c r="B1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1" t="s">
         <v>331</v>
-      </c>
-      <c r="C1" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="2" spans="2:3">

</xml_diff>